<commit_message>
added NO column in es_mx locale
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
+++ b/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEC_31\OVWMigration\docs\OVW Sheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="5" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ja_jp" sheetId="48" r:id="rId1"/>
@@ -66,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11975" uniqueCount="2517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12002" uniqueCount="2517">
   <si>
     <t>products</t>
   </si>
@@ -8324,7 +8329,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -15133,7 +15138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -47880,8 +47885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28:E57"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47891,7 +47896,7 @@
     <col min="3" max="3" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>196</v>
       </c>
@@ -47904,8 +47909,11 @@
       <c r="D1" s="32" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="218" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>197</v>
       </c>
@@ -47918,8 +47926,11 @@
       <c r="D2" s="32" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="218" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>198</v>
       </c>
@@ -47932,8 +47943,11 @@
       <c r="D3" s="32" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="218" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>199</v>
       </c>
@@ -47946,8 +47960,11 @@
       <c r="D4" s="32" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="218" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>200</v>
       </c>
@@ -47960,8 +47977,11 @@
       <c r="D5" s="32" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="218" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>201</v>
       </c>
@@ -47974,8 +47994,11 @@
       <c r="D6" s="32" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="218" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>203</v>
       </c>
@@ -47988,8 +48011,11 @@
       <c r="D7" s="32" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="218" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>204</v>
       </c>
@@ -48002,8 +48028,11 @@
       <c r="D8" s="32" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="218" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>205</v>
       </c>
@@ -48016,8 +48045,11 @@
       <c r="D9" s="32" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="218" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>207</v>
       </c>
@@ -48030,8 +48062,11 @@
       <c r="D10" s="32" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="218" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>208</v>
       </c>
@@ -48044,8 +48079,11 @@
       <c r="D11" s="32" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="218" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
         <v>209</v>
       </c>
@@ -48058,8 +48096,11 @@
       <c r="D12" s="32" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="218" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>210</v>
       </c>
@@ -48072,8 +48113,11 @@
       <c r="D13" s="32" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="218" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
         <v>211</v>
       </c>
@@ -48086,8 +48130,11 @@
       <c r="D14" s="32" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="218" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>212</v>
       </c>
@@ -48100,8 +48147,11 @@
       <c r="D15" s="32" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="218" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
         <v>215</v>
       </c>
@@ -48113,6 +48163,9 @@
       </c>
       <c r="D16" s="32" t="s">
         <v>21</v>
+      </c>
+      <c r="E16" s="218" t="s">
+        <v>2075</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -48128,6 +48181,9 @@
       <c r="D17" s="32" t="s">
         <v>21</v>
       </c>
+      <c r="E17" s="218" t="s">
+        <v>2075</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
@@ -48142,6 +48198,9 @@
       <c r="D18" s="32" t="s">
         <v>21</v>
       </c>
+      <c r="E18" s="218" t="s">
+        <v>2075</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
@@ -48156,6 +48215,9 @@
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
+      <c r="E19" s="218" t="s">
+        <v>2075</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
@@ -48170,6 +48232,9 @@
       <c r="D20" s="32" t="s">
         <v>21</v>
       </c>
+      <c r="E20" s="218" t="s">
+        <v>2075</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
@@ -48184,6 +48249,9 @@
       <c r="D21" s="32" t="s">
         <v>21</v>
       </c>
+      <c r="E21" s="218" t="s">
+        <v>2075</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
@@ -48198,6 +48266,9 @@
       <c r="D22" s="32" t="s">
         <v>21</v>
       </c>
+      <c r="E22" s="218" t="s">
+        <v>2075</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
@@ -48212,6 +48283,9 @@
       <c r="D23" s="32" t="s">
         <v>21</v>
       </c>
+      <c r="E23" s="218" t="s">
+        <v>2075</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
@@ -48226,6 +48300,9 @@
       <c r="D24" s="32" t="s">
         <v>21</v>
       </c>
+      <c r="E24" s="218" t="s">
+        <v>2075</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
@@ -48240,6 +48317,9 @@
       <c r="D25" s="36" t="s">
         <v>21</v>
       </c>
+      <c r="E25" s="218" t="s">
+        <v>2075</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="34" t="s">
@@ -48254,6 +48334,9 @@
       <c r="D26" s="36" t="s">
         <v>21</v>
       </c>
+      <c r="E26" s="218" t="s">
+        <v>2075</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="34" t="s">
@@ -48267,6 +48350,9 @@
       </c>
       <c r="D27" s="36" t="s">
         <v>0</v>
+      </c>
+      <c r="E27" s="218" t="s">
+        <v>2075</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added webvar7 5-urls in OVWDemo_ALL_URLS.xlsx
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
+++ b/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_OVWMig\jan_13\OVWMigration\docs\OVW Sheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11010" activeTab="46"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11010" firstSheet="34" activeTab="41"/>
   </bookViews>
   <sheets>
     <sheet name="ja_jp" sheetId="48" r:id="rId1"/>
@@ -66,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14331" uniqueCount="2840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14701" uniqueCount="2919">
   <si>
     <t>products</t>
   </si>
@@ -8586,6 +8591,243 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/IN/products/unified_computing/services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/solution/industries/energy/index.html</t>
+  </si>
+  <si>
+    <t>industries</t>
+  </si>
+  <si>
+    <t>energy-webvar7</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/solution/industries/retail/index.html</t>
+  </si>
+  <si>
+    <t>retail-webvar7</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/solution/industries/government/index.html</t>
+  </si>
+  <si>
+    <t>government-webvar7</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/solution/industries/manufacturing/index.html</t>
+  </si>
+  <si>
+    <t>manufacturing-webvar7</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/solution/industries/financial/index.html</t>
+  </si>
+  <si>
+    <t>financial-services-webvar7</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CN/solutions/strategy/energy/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CN/solutions/strategy/retail/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CN/solutions/strategy/government/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CN/solutions/strategy/manufacturing/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CN/solutions/strategy/financial/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/cisco/web/UK/solutions/strategy/energy/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/cisco/web/UK/solutions/strategy/retail/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/cisco/web/UK/solutions/strategy/manufacturing/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/cisco/web/UK/solutions/strategy/financial/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/strategy/energy/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/strategy/retail/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/strategy/government/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/strategy/manufacturing/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/strategy/financial/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/LA/soluciones/strategy/energy/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/LA/soluciones/strategy/retail/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/LA/soluciones/strategy/government/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/LA/soluciones/strategy/manufacturing/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/LA/soluciones/strategy/financial/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/solucoes/strategy/energy/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/solucoes/strategy/retail/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/solucoes/strategy/government/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/solucoes/strategy/manufacturing/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/solucoes/strategy/financial/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/ar/solutions/strategy/energy/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/ar/solutions/strategy/retail/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/ar/solutions/strategy/government/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/ar/solutions/strategy/manufacturing/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/ar/solutions/strategy/financial/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/strategy/energy/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/strategy/retail/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/strategy/government/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/strategy/manufacturing/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/strategy/financial/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FR/solutions/strategy/energy/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FR/solutions/strategy/retail/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FR/solutions/strategy/government/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FR/solutions/strategy/manufacturing/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FR/solutions/strategy/financial/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/solutions/strategy/energy/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/solutions/strategy/retail/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/solutions/strategy/government/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/solutions/strategy/manufacturing/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/solutions/strategy/financial/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/solutions/strategy/energy/index_fr.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/solutions/strategy/retail/index_fr.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/solutions/strategy/government/index_fr.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/solutions/strategy/financial/index_fr.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ANZ/netsol/strategy/energy/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ANZ/netsol/strategy/retail/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ANZ/netsol/strategy/government/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ANZ/netsol/strategy/manufacturing/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ANZ/netsol/strategy/financial/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IN/solutions/strategy/energy/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IN/solutions/strategy/retail/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IN/solutions/strategy/government/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IN/solutions/strategy/manufacturing/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IN/solutions/strategy/financial/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/KR/networking/strategy/energy/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/KR/networking/strategy/retail/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/KR/networking/strategy/government/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/KR/networking/strategy/manufacturing/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/KR/networking/strategy/financial/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/solutions/strategy/energy/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/solutions/strategy/retail/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/solutions/strategy/government/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/solutions/strategy/manufacturing/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/solutions/strategy/financial/index.html</t>
   </si>
 </sst>
 </file>
@@ -9339,7 +9581,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9347,10 +9589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A70" sqref="A70:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10517,6 +10759,91 @@
       </c>
       <c r="D69" s="215"/>
       <c r="E69" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="215" t="s">
+        <v>2840</v>
+      </c>
+      <c r="B70" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C70" s="215" t="s">
+        <v>2842</v>
+      </c>
+      <c r="D70" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="215" t="s">
+        <v>2843</v>
+      </c>
+      <c r="B71" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C71" s="215" t="s">
+        <v>2844</v>
+      </c>
+      <c r="D71" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="215" t="s">
+        <v>2845</v>
+      </c>
+      <c r="B72" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C72" s="215" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D72" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="215" t="s">
+        <v>2847</v>
+      </c>
+      <c r="B73" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C73" s="215" t="s">
+        <v>2848</v>
+      </c>
+      <c r="D73" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="215" t="s">
+        <v>2849</v>
+      </c>
+      <c r="B74" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C74" s="215" t="s">
+        <v>2850</v>
+      </c>
+      <c r="D74" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -10598,10 +10925,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:E72"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73:E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11820,6 +12147,91 @@
       </c>
       <c r="D72" s="215"/>
       <c r="E72" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="215" t="s">
+        <v>2890</v>
+      </c>
+      <c r="B73" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C73" s="215" t="s">
+        <v>2842</v>
+      </c>
+      <c r="D73" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="215" t="s">
+        <v>2891</v>
+      </c>
+      <c r="B74" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C74" s="215" t="s">
+        <v>2844</v>
+      </c>
+      <c r="D74" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="215" t="s">
+        <v>2892</v>
+      </c>
+      <c r="B75" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C75" s="215" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D75" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="215" t="s">
+        <v>2893</v>
+      </c>
+      <c r="B76" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C76" s="215" t="s">
+        <v>2848</v>
+      </c>
+      <c r="D76" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="215" t="s">
+        <v>2894</v>
+      </c>
+      <c r="B77" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C77" s="215" t="s">
+        <v>2850</v>
+      </c>
+      <c r="D77" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -11904,10 +12316,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13142,6 +13554,91 @@
       </c>
       <c r="D73" s="215"/>
       <c r="E73" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="215" t="s">
+        <v>2895</v>
+      </c>
+      <c r="B74" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C74" s="215" t="s">
+        <v>2842</v>
+      </c>
+      <c r="D74" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="215" t="s">
+        <v>2896</v>
+      </c>
+      <c r="B75" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C75" s="215" t="s">
+        <v>2844</v>
+      </c>
+      <c r="D75" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="215" t="s">
+        <v>2897</v>
+      </c>
+      <c r="B76" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C76" s="215" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D76" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="215" t="s">
+        <v>2893</v>
+      </c>
+      <c r="B77" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C77" s="215" t="s">
+        <v>2848</v>
+      </c>
+      <c r="D77" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="215" t="s">
+        <v>2898</v>
+      </c>
+      <c r="B78" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C78" s="215" t="s">
+        <v>2850</v>
+      </c>
+      <c r="D78" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -13226,10 +13723,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:E72"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73:E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14444,6 +14941,91 @@
       </c>
       <c r="D72" s="215"/>
       <c r="E72" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="215" t="s">
+        <v>2899</v>
+      </c>
+      <c r="B73" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C73" s="215" t="s">
+        <v>2842</v>
+      </c>
+      <c r="D73" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="215" t="s">
+        <v>2900</v>
+      </c>
+      <c r="B74" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C74" s="215" t="s">
+        <v>2844</v>
+      </c>
+      <c r="D74" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="215" t="s">
+        <v>2901</v>
+      </c>
+      <c r="B75" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C75" s="215" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D75" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="215" t="s">
+        <v>2902</v>
+      </c>
+      <c r="B76" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C76" s="215" t="s">
+        <v>2848</v>
+      </c>
+      <c r="D76" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="215" t="s">
+        <v>2903</v>
+      </c>
+      <c r="B77" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C77" s="215" t="s">
+        <v>2850</v>
+      </c>
+      <c r="D77" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -14525,10 +15107,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15780,6 +16362,91 @@
       </c>
       <c r="D74" s="215"/>
       <c r="E74" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="215" t="s">
+        <v>2904</v>
+      </c>
+      <c r="B75" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C75" s="215" t="s">
+        <v>2842</v>
+      </c>
+      <c r="D75" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="215" t="s">
+        <v>2905</v>
+      </c>
+      <c r="B76" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C76" s="215" t="s">
+        <v>2844</v>
+      </c>
+      <c r="D76" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="215" t="s">
+        <v>2906</v>
+      </c>
+      <c r="B77" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C77" s="215" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D77" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="215" t="s">
+        <v>2907</v>
+      </c>
+      <c r="B78" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C78" s="215" t="s">
+        <v>2848</v>
+      </c>
+      <c r="D78" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="215" t="s">
+        <v>2908</v>
+      </c>
+      <c r="B79" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C79" s="215" t="s">
+        <v>2850</v>
+      </c>
+      <c r="D79" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E79" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -15866,10 +16533,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:E74"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17121,6 +17788,91 @@
       </c>
       <c r="D74" s="215"/>
       <c r="E74" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="215" t="s">
+        <v>2909</v>
+      </c>
+      <c r="B75" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C75" s="215" t="s">
+        <v>2842</v>
+      </c>
+      <c r="D75" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="215" t="s">
+        <v>2910</v>
+      </c>
+      <c r="B76" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C76" s="215" t="s">
+        <v>2844</v>
+      </c>
+      <c r="D76" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="215" t="s">
+        <v>2911</v>
+      </c>
+      <c r="B77" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C77" s="215" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D77" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="215" t="s">
+        <v>2912</v>
+      </c>
+      <c r="B78" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C78" s="215" t="s">
+        <v>2848</v>
+      </c>
+      <c r="D78" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="215" t="s">
+        <v>2913</v>
+      </c>
+      <c r="B79" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C79" s="215" t="s">
+        <v>2850</v>
+      </c>
+      <c r="D79" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E79" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -22561,10 +23313,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23732,6 +24484,91 @@
       </c>
       <c r="D69" s="215"/>
       <c r="E69" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="215" t="s">
+        <v>2851</v>
+      </c>
+      <c r="B70" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C70" s="215" t="s">
+        <v>2842</v>
+      </c>
+      <c r="D70" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="215" t="s">
+        <v>2852</v>
+      </c>
+      <c r="B71" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C71" s="215" t="s">
+        <v>2844</v>
+      </c>
+      <c r="D71" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="215" t="s">
+        <v>2853</v>
+      </c>
+      <c r="B72" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C72" s="215" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D72" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="215" t="s">
+        <v>2854</v>
+      </c>
+      <c r="B73" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C73" s="215" t="s">
+        <v>2848</v>
+      </c>
+      <c r="D73" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="215" t="s">
+        <v>2855</v>
+      </c>
+      <c r="B74" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C74" s="215" t="s">
+        <v>2850</v>
+      </c>
+      <c r="D74" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -34941,10 +35778,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:E73"/>
+      <selection activeCell="A74" sqref="A74:E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36179,6 +37016,74 @@
       </c>
       <c r="D73" s="215"/>
       <c r="E73" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="215" t="s">
+        <v>2856</v>
+      </c>
+      <c r="B74" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C74" s="215" t="s">
+        <v>2842</v>
+      </c>
+      <c r="D74" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="215" t="s">
+        <v>2857</v>
+      </c>
+      <c r="B75" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C75" s="215" t="s">
+        <v>2844</v>
+      </c>
+      <c r="D75" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="215" t="s">
+        <v>2858</v>
+      </c>
+      <c r="B76" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C76" s="215" t="s">
+        <v>2848</v>
+      </c>
+      <c r="D76" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="215" t="s">
+        <v>2859</v>
+      </c>
+      <c r="B77" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C77" s="215" t="s">
+        <v>2850</v>
+      </c>
+      <c r="D77" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -44878,10 +45783,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:E73"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46116,6 +47021,91 @@
       </c>
       <c r="D73" s="215"/>
       <c r="E73" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="215" t="s">
+        <v>2860</v>
+      </c>
+      <c r="B74" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C74" s="215" t="s">
+        <v>2842</v>
+      </c>
+      <c r="D74" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="215" t="s">
+        <v>2861</v>
+      </c>
+      <c r="B75" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C75" s="215" t="s">
+        <v>2844</v>
+      </c>
+      <c r="D75" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="215" t="s">
+        <v>2862</v>
+      </c>
+      <c r="B76" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C76" s="215" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D76" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="215" t="s">
+        <v>2863</v>
+      </c>
+      <c r="B77" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C77" s="215" t="s">
+        <v>2848</v>
+      </c>
+      <c r="D77" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="215" t="s">
+        <v>2864</v>
+      </c>
+      <c r="B78" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C78" s="215" t="s">
+        <v>2850</v>
+      </c>
+      <c r="D78" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -47814,10 +48804,10 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:E73"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49052,6 +50042,91 @@
       </c>
       <c r="D73" s="215"/>
       <c r="E73" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="215" t="s">
+        <v>2914</v>
+      </c>
+      <c r="B74" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C74" s="215" t="s">
+        <v>2842</v>
+      </c>
+      <c r="D74" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="215" t="s">
+        <v>2915</v>
+      </c>
+      <c r="B75" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C75" s="215" t="s">
+        <v>2844</v>
+      </c>
+      <c r="D75" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="215" t="s">
+        <v>2916</v>
+      </c>
+      <c r="B76" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C76" s="215" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D76" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="215" t="s">
+        <v>2917</v>
+      </c>
+      <c r="B77" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C77" s="215" t="s">
+        <v>2848</v>
+      </c>
+      <c r="D77" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="215" t="s">
+        <v>2918</v>
+      </c>
+      <c r="B78" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C78" s="215" t="s">
+        <v>2850</v>
+      </c>
+      <c r="D78" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -54004,7 +55079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -55718,10 +56793,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:E72"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56936,6 +58011,91 @@
       </c>
       <c r="D72" s="215"/>
       <c r="E72" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="215" t="s">
+        <v>2865</v>
+      </c>
+      <c r="B73" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C73" s="215" t="s">
+        <v>2842</v>
+      </c>
+      <c r="D73" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="215" t="s">
+        <v>2866</v>
+      </c>
+      <c r="B74" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C74" s="215" t="s">
+        <v>2844</v>
+      </c>
+      <c r="D74" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="215" t="s">
+        <v>2867</v>
+      </c>
+      <c r="B75" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C75" s="215" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D75" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="215" t="s">
+        <v>2868</v>
+      </c>
+      <c r="B76" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C76" s="215" t="s">
+        <v>2848</v>
+      </c>
+      <c r="D76" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="215" t="s">
+        <v>2869</v>
+      </c>
+      <c r="B77" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C77" s="215" t="s">
+        <v>2850</v>
+      </c>
+      <c r="D77" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -57018,10 +58178,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:E74"/>
+      <selection activeCell="A75" sqref="A75:E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58274,6 +59434,91 @@
       </c>
       <c r="D74" s="215"/>
       <c r="E74" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="215" t="s">
+        <v>2870</v>
+      </c>
+      <c r="B75" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C75" s="215" t="s">
+        <v>2842</v>
+      </c>
+      <c r="D75" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="215" t="s">
+        <v>2871</v>
+      </c>
+      <c r="B76" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C76" s="215" t="s">
+        <v>2844</v>
+      </c>
+      <c r="D76" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="215" t="s">
+        <v>2872</v>
+      </c>
+      <c r="B77" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C77" s="215" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D77" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="215" t="s">
+        <v>2873</v>
+      </c>
+      <c r="B78" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C78" s="215" t="s">
+        <v>2848</v>
+      </c>
+      <c r="D78" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="215" t="s">
+        <v>2874</v>
+      </c>
+      <c r="B79" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C79" s="215" t="s">
+        <v>2850</v>
+      </c>
+      <c r="D79" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E79" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -58361,10 +59606,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:E73"/>
+      <selection activeCell="A74" sqref="A74:E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59600,6 +60845,91 @@
       </c>
       <c r="D73" s="215"/>
       <c r="E73" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="215" t="s">
+        <v>2875</v>
+      </c>
+      <c r="B74" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C74" s="215" t="s">
+        <v>2842</v>
+      </c>
+      <c r="D74" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="215" t="s">
+        <v>2876</v>
+      </c>
+      <c r="B75" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C75" s="215" t="s">
+        <v>2844</v>
+      </c>
+      <c r="D75" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="215" t="s">
+        <v>2877</v>
+      </c>
+      <c r="B76" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C76" s="215" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D76" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="215" t="s">
+        <v>2878</v>
+      </c>
+      <c r="B77" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C77" s="215" t="s">
+        <v>2848</v>
+      </c>
+      <c r="D77" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="215" t="s">
+        <v>2879</v>
+      </c>
+      <c r="B78" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C78" s="215" t="s">
+        <v>2850</v>
+      </c>
+      <c r="D78" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -59685,10 +61015,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:E72"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73:E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60907,6 +62237,91 @@
       </c>
       <c r="D72" s="215"/>
       <c r="E72" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="215" t="s">
+        <v>2880</v>
+      </c>
+      <c r="B73" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C73" s="215" t="s">
+        <v>2842</v>
+      </c>
+      <c r="D73" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="215" t="s">
+        <v>2881</v>
+      </c>
+      <c r="B74" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C74" s="215" t="s">
+        <v>2844</v>
+      </c>
+      <c r="D74" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="215" t="s">
+        <v>2882</v>
+      </c>
+      <c r="B75" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C75" s="215" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D75" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="215" t="s">
+        <v>2883</v>
+      </c>
+      <c r="B76" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C76" s="215" t="s">
+        <v>2848</v>
+      </c>
+      <c r="D76" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="215" t="s">
+        <v>2884</v>
+      </c>
+      <c r="B77" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C77" s="215" t="s">
+        <v>2850</v>
+      </c>
+      <c r="D77" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -60989,10 +62404,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:E73"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62228,6 +63643,91 @@
       </c>
       <c r="D73" s="215"/>
       <c r="E73" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="215" t="s">
+        <v>2885</v>
+      </c>
+      <c r="B74" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C74" s="215" t="s">
+        <v>2842</v>
+      </c>
+      <c r="D74" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="215" t="s">
+        <v>2886</v>
+      </c>
+      <c r="B75" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C75" s="215" t="s">
+        <v>2844</v>
+      </c>
+      <c r="D75" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="215" t="s">
+        <v>2887</v>
+      </c>
+      <c r="B76" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C76" s="215" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D76" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="215" t="s">
+        <v>2888</v>
+      </c>
+      <c r="B77" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C77" s="215" t="s">
+        <v>2848</v>
+      </c>
+      <c r="D77" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="215" t="s">
+        <v>2889</v>
+      </c>
+      <c r="B78" s="215" t="s">
+        <v>2841</v>
+      </c>
+      <c r="C78" s="215" t="s">
+        <v>2850</v>
+      </c>
+      <c r="D78" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" s="215" t="s">
         <v>2075</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the OVWDemo ALL URLs sheet.
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
+++ b/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW Migration\OVWMigration\docs\OVW Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdevalka\OVW Migration Project\Daily Checkout\13 Jan\Evening\OVWMigration\docs\OVW Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11010" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11010"/>
   </bookViews>
   <sheets>
     <sheet name="ja_jp" sheetId="48" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15039" uniqueCount="3001">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15274" uniqueCount="3049">
   <si>
     <t>products</t>
   </si>
@@ -8845,9 +8845,6 @@
     <t>managed-cloud-services-pswebvar5</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>http://www.cisco.com/web/JP/solution/trends/cloud/private-cloud-hybrid-cloud-solutions.html</t>
   </si>
   <si>
@@ -9074,6 +9071,153 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/BR/solucoes/collaboration/architecture.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>midsize</t>
+  </si>
+  <si>
+    <t>products-fsvar4</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/cisco/web/UK/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/LA/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/ar/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FR/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/midsize/products_solutions_fr.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ANZ/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IN/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/KR/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/SG/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/NO/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PL/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PT/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RO/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ZA/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ES/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/SE/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CH/fr/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CH/de/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TR/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/UA/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/UA/uk/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/HK/tc/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/HK/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TW/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/EA/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IL/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/GR/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/nl/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FI/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BG/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CZ/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DK/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/EA/midsize/FR/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/HU/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IT/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/NL/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TH/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/AT/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ID/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/fr/midsize/products_solutions.html</t>
   </si>
 </sst>
 </file>
@@ -9835,10 +9979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:E77"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11122,24 +11266,41 @@
         <v>21</v>
       </c>
       <c r="E76" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="206" t="s">
-        <v>2925</v>
+        <v>2924</v>
       </c>
       <c r="B77" s="215" t="s">
         <v>2649</v>
       </c>
       <c r="C77" s="215" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="D77" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E77" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="215" t="s">
+        <v>3000</v>
+      </c>
+      <c r="B78" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C78" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D78" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" s="217" t="s">
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -11222,10 +11383,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:E80"/>
+      <selection activeCell="B81" sqref="B81:E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12534,7 +12695,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="205" t="s">
-        <v>2951</v>
+        <v>2950</v>
       </c>
       <c r="B78" s="215"/>
       <c r="C78" s="215" t="s">
@@ -12549,7 +12710,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="206" t="s">
-        <v>2952</v>
+        <v>2951</v>
       </c>
       <c r="B79" s="215" t="s">
         <v>2649</v>
@@ -12561,24 +12722,41 @@
         <v>21</v>
       </c>
       <c r="E79" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="206" t="s">
-        <v>2953</v>
+        <v>2952</v>
       </c>
       <c r="B80" s="215" t="s">
         <v>2649</v>
       </c>
       <c r="C80" s="215" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="D80" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E80" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="206" t="s">
+        <v>3010</v>
+      </c>
+      <c r="B81" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C81" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D81" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E81" s="217" t="s">
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -12657,6 +12835,7 @@
     <hyperlink ref="A72" r:id="rId72"/>
     <hyperlink ref="A79" r:id="rId73"/>
     <hyperlink ref="A80" r:id="rId74"/>
+    <hyperlink ref="A81" r:id="rId75"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12664,10 +12843,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:E81"/>
+      <selection activeCell="B82" sqref="B82:E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13992,7 +14171,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="206" t="s">
-        <v>2954</v>
+        <v>2953</v>
       </c>
       <c r="B79" s="215"/>
       <c r="C79" s="215" t="s">
@@ -14007,7 +14186,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="206" t="s">
-        <v>2955</v>
+        <v>2954</v>
       </c>
       <c r="B80" s="215" t="s">
         <v>2649</v>
@@ -14019,24 +14198,41 @@
         <v>21</v>
       </c>
       <c r="E80" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="206" t="s">
-        <v>2956</v>
+        <v>2955</v>
       </c>
       <c r="B81" s="215" t="s">
         <v>2649</v>
       </c>
       <c r="C81" s="215" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="D81" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E81" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="206" t="s">
+        <v>3011</v>
+      </c>
+      <c r="B82" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C82" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D82" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E82" s="217" t="s">
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -14116,6 +14312,7 @@
     <hyperlink ref="A79" r:id="rId73"/>
     <hyperlink ref="A80" r:id="rId74"/>
     <hyperlink ref="A81" r:id="rId75"/>
+    <hyperlink ref="A82" r:id="rId76"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14123,10 +14320,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:E80"/>
+      <selection activeCell="B81" sqref="B81:E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15431,7 +15628,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
-        <v>2957</v>
+        <v>2956</v>
       </c>
       <c r="B78" s="215"/>
       <c r="C78" s="215" t="s">
@@ -15446,7 +15643,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="228" t="s">
-        <v>2958</v>
+        <v>2957</v>
       </c>
       <c r="B79" s="215" t="s">
         <v>2649</v>
@@ -15458,24 +15655,41 @@
         <v>21</v>
       </c>
       <c r="E79" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="228" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="B80" s="215" t="s">
         <v>2649</v>
       </c>
       <c r="C80" s="215" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="D80" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E80" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="206" t="s">
+        <v>3012</v>
+      </c>
+      <c r="B81" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C81" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D81" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E81" s="217" t="s">
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -15552,6 +15766,7 @@
     <hyperlink ref="A78" r:id="rId70"/>
     <hyperlink ref="A79" r:id="rId71"/>
     <hyperlink ref="A80" r:id="rId72"/>
+    <hyperlink ref="A81" r:id="rId73"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15559,10 +15774,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80:E82"/>
+      <selection activeCell="B83" sqref="B83:E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16904,7 +17119,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="199" t="s">
-        <v>2960</v>
+        <v>2959</v>
       </c>
       <c r="B80" s="215"/>
       <c r="C80" s="215" t="s">
@@ -16919,7 +17134,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="206" t="s">
-        <v>2961</v>
+        <v>2960</v>
       </c>
       <c r="B81" s="215" t="s">
         <v>2649</v>
@@ -16931,24 +17146,41 @@
         <v>21</v>
       </c>
       <c r="E81" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="206" t="s">
-        <v>2962</v>
+        <v>2961</v>
       </c>
       <c r="B82" s="215" t="s">
         <v>2649</v>
       </c>
       <c r="C82" s="215" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="D82" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E82" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="206" t="s">
+        <v>3013</v>
+      </c>
+      <c r="B83" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C83" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D83" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="217" t="s">
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -17029,18 +17261,19 @@
     <hyperlink ref="A81" r:id="rId74"/>
     <hyperlink ref="A82" r:id="rId75"/>
     <hyperlink ref="A80" r:id="rId76"/>
+    <hyperlink ref="A83" r:id="rId77"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId77"/>
+  <pageSetup orientation="portrait" r:id="rId78"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80:E82"/>
+      <selection activeCell="B83" sqref="B83:E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18382,7 +18615,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="205" t="s">
-        <v>2963</v>
+        <v>2962</v>
       </c>
       <c r="B80" s="215"/>
       <c r="C80" s="215" t="s">
@@ -18397,7 +18630,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="205" t="s">
-        <v>2964</v>
+        <v>2963</v>
       </c>
       <c r="B81" s="215" t="s">
         <v>2649</v>
@@ -18409,24 +18642,41 @@
         <v>21</v>
       </c>
       <c r="E81" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="205" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="B82" s="215" t="s">
         <v>2649</v>
       </c>
       <c r="C82" s="215" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="D82" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E82" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="206" t="s">
+        <v>3014</v>
+      </c>
+      <c r="B83" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C83" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D83" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="217" t="s">
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -18506,6 +18756,7 @@
     <hyperlink ref="A73" r:id="rId73"/>
     <hyperlink ref="A81" r:id="rId74"/>
     <hyperlink ref="A82" r:id="rId75"/>
+    <hyperlink ref="A83" r:id="rId76"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18513,10 +18764,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70:E70"/>
+      <selection activeCell="B71" sqref="B71:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19688,7 +19939,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="205" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="B70" s="215"/>
       <c r="C70" s="215" t="s">
@@ -19698,6 +19949,23 @@
         <v>2921</v>
       </c>
       <c r="E70" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="205" t="s">
+        <v>3015</v>
+      </c>
+      <c r="B71" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C71" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D71" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -19771,6 +20039,7 @@
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
     <hyperlink ref="A68" r:id="rId68"/>
+    <hyperlink ref="A71" r:id="rId69"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19781,7 +20050,7 @@
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:E68"/>
+      <selection activeCell="B69" sqref="B69:E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20923,7 +21192,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="206" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="B68" s="215"/>
       <c r="C68" s="215" t="s">
@@ -20937,10 +21206,21 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="206"/>
-      <c r="B69" s="215"/>
-      <c r="C69" s="215"/>
-      <c r="D69" s="215"/>
+      <c r="A69" s="206" t="s">
+        <v>3016</v>
+      </c>
+      <c r="B69" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C69" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D69" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E69" s="217" t="s">
+        <v>2075</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="206"/>
@@ -21040,6 +21320,7 @@
     <hyperlink ref="A65" r:id="rId64"/>
     <hyperlink ref="A66" r:id="rId65"/>
     <hyperlink ref="A67" r:id="rId66"/>
+    <hyperlink ref="A69" r:id="rId67"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21047,10 +21328,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:E69"/>
+      <selection activeCell="B70" sqref="B70:E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22202,7 +22483,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="206" t="s">
-        <v>2968</v>
+        <v>2967</v>
       </c>
       <c r="C69" s="215" t="s">
         <v>2920</v>
@@ -22211,6 +22492,23 @@
         <v>2921</v>
       </c>
       <c r="E69" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="206" t="s">
+        <v>3017</v>
+      </c>
+      <c r="B70" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C70" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D70" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -22282,6 +22580,7 @@
     <hyperlink ref="A65" r:id="rId64"/>
     <hyperlink ref="A66" r:id="rId65"/>
     <hyperlink ref="A67" r:id="rId66"/>
+    <hyperlink ref="A70" r:id="rId67"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22289,10 +22588,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:E68"/>
+      <selection activeCell="B69" sqref="B69:E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23432,7 +23731,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="205" t="s">
-        <v>2969</v>
+        <v>2968</v>
       </c>
       <c r="C68" s="215" t="s">
         <v>2920</v>
@@ -23441,6 +23740,23 @@
         <v>2921</v>
       </c>
       <c r="E68" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="205" t="s">
+        <v>3018</v>
+      </c>
+      <c r="B69" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C69" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D69" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E69" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -23514,6 +23830,7 @@
     <hyperlink ref="A65" r:id="rId66"/>
     <hyperlink ref="A66" r:id="rId67"/>
     <hyperlink ref="A67" r:id="rId68"/>
+    <hyperlink ref="A69" r:id="rId69"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -23524,7 +23841,7 @@
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:E20"/>
+      <selection activeCell="B21" sqref="B21:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23851,7 +24168,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="206" t="s">
-        <v>2970</v>
+        <v>2969</v>
       </c>
       <c r="B20" s="215"/>
       <c r="C20" s="215" t="s">
@@ -23861,6 +24178,23 @@
         <v>2921</v>
       </c>
       <c r="E20" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="206" t="s">
+        <v>3019</v>
+      </c>
+      <c r="B21" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C21" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D21" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -23928,6 +24262,7 @@
     <hyperlink ref="A17" r:id="rId18"/>
     <hyperlink ref="A18" r:id="rId19"/>
     <hyperlink ref="A19" r:id="rId20"/>
+    <hyperlink ref="A21" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -25196,7 +25531,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="216" t="s">
-        <v>2927</v>
+        <v>2926</v>
       </c>
       <c r="B75" s="215"/>
       <c r="C75" s="215" t="s">
@@ -25211,7 +25546,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="205" t="s">
-        <v>2928</v>
+        <v>2927</v>
       </c>
       <c r="B76" s="215" t="s">
         <v>2649</v>
@@ -25223,24 +25558,24 @@
         <v>21</v>
       </c>
       <c r="E76" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="205" t="s">
-        <v>2929</v>
+        <v>2928</v>
       </c>
       <c r="B77" s="215" t="s">
         <v>2649</v>
       </c>
       <c r="C77" s="215" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="D77" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E77" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -25322,10 +25657,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63:E63"/>
+      <selection activeCell="B64" sqref="B64:E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26378,7 +26713,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="206" t="s">
-        <v>2971</v>
+        <v>2970</v>
       </c>
       <c r="B63" s="215"/>
       <c r="C63" s="215" t="s">
@@ -26388,6 +26723,23 @@
         <v>2921</v>
       </c>
       <c r="E63" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="206" t="s">
+        <v>3020</v>
+      </c>
+      <c r="B64" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C64" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D64" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E64" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -26447,6 +26799,7 @@
     <hyperlink ref="A59" r:id="rId52"/>
     <hyperlink ref="A60" r:id="rId53"/>
     <hyperlink ref="A61" r:id="rId54"/>
+    <hyperlink ref="A64" r:id="rId55"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -26454,10 +26807,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:E69"/>
+      <selection activeCell="B70" sqref="B70:E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27608,7 +27961,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="205" t="s">
-        <v>2972</v>
+        <v>2971</v>
       </c>
       <c r="C69" s="215" t="s">
         <v>2920</v>
@@ -27617,6 +27970,23 @@
         <v>2921</v>
       </c>
       <c r="E69" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="206" t="s">
+        <v>3021</v>
+      </c>
+      <c r="B70" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C70" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D70" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -27689,6 +28059,7 @@
     <hyperlink ref="A65" r:id="rId65"/>
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
+    <hyperlink ref="A70" r:id="rId68"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -27696,10 +28067,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:E68"/>
+      <selection activeCell="B69" sqref="B69:E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28839,7 +29210,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="206" t="s">
-        <v>2973</v>
+        <v>2972</v>
       </c>
       <c r="C68" s="215" t="s">
         <v>2920</v>
@@ -28848,6 +29219,23 @@
         <v>2921</v>
       </c>
       <c r="E68" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="206" t="s">
+        <v>3022</v>
+      </c>
+      <c r="B69" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C69" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D69" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E69" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -28920,6 +29308,7 @@
     <hyperlink ref="A65" r:id="rId65"/>
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
+    <hyperlink ref="A69" r:id="rId68"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28927,10 +29316,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:E67"/>
+      <selection activeCell="B68" sqref="B68:E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30053,7 +30442,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="205" t="s">
-        <v>2974</v>
+        <v>2973</v>
       </c>
       <c r="C67" s="215" t="s">
         <v>2920</v>
@@ -30062,6 +30451,23 @@
         <v>2921</v>
       </c>
       <c r="E67" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="205" t="s">
+        <v>3023</v>
+      </c>
+      <c r="B68" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C68" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D68" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E68" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -30133,6 +30539,7 @@
     <hyperlink ref="A64" r:id="rId64"/>
     <hyperlink ref="A65" r:id="rId65"/>
     <hyperlink ref="A66" r:id="rId66"/>
+    <hyperlink ref="A68" r:id="rId67"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -30140,10 +30547,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:E67"/>
+      <selection activeCell="B68" sqref="B68:E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31266,7 +31673,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="205" t="s">
-        <v>2974</v>
+        <v>2973</v>
       </c>
       <c r="C67" s="215" t="s">
         <v>2920</v>
@@ -31275,6 +31682,23 @@
         <v>2921</v>
       </c>
       <c r="E67" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="205" t="s">
+        <v>3024</v>
+      </c>
+      <c r="B68" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C68" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D68" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E68" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -31347,6 +31771,7 @@
     <hyperlink ref="A64" r:id="rId65"/>
     <hyperlink ref="A65" r:id="rId66"/>
     <hyperlink ref="A66" r:id="rId67"/>
+    <hyperlink ref="A68" r:id="rId68"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -31354,10 +31779,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:E69"/>
+      <selection activeCell="B70" sqref="B70:E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32508,7 +32933,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="206" t="s">
-        <v>2975</v>
+        <v>2974</v>
       </c>
       <c r="C69" s="215" t="s">
         <v>2920</v>
@@ -32517,6 +32942,23 @@
         <v>2921</v>
       </c>
       <c r="E69" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="206" t="s">
+        <v>3025</v>
+      </c>
+      <c r="B70" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C70" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D70" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -32589,6 +33031,7 @@
     <hyperlink ref="A65" r:id="rId65"/>
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
+    <hyperlink ref="A70" r:id="rId68"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -32596,10 +33039,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:E65"/>
+      <selection activeCell="B66" sqref="B66:E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33682,7 +34125,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="206" t="s">
-        <v>2976</v>
+        <v>2975</v>
       </c>
       <c r="C65" s="215" t="s">
         <v>2920</v>
@@ -33691,6 +34134,23 @@
         <v>2921</v>
       </c>
       <c r="E65" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="206" t="s">
+        <v>3026</v>
+      </c>
+      <c r="B66" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C66" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D66" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -33759,6 +34219,7 @@
     <hyperlink ref="A61" r:id="rId61"/>
     <hyperlink ref="A62" r:id="rId62"/>
     <hyperlink ref="A63" r:id="rId63"/>
+    <hyperlink ref="A66" r:id="rId64"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33766,10 +34227,10 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:E20"/>
+      <selection activeCell="B21" sqref="B21:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34095,7 +34556,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="205" t="s">
-        <v>2977</v>
+        <v>2976</v>
       </c>
       <c r="B20" s="215"/>
       <c r="C20" s="215" t="s">
@@ -34105,6 +34566,23 @@
         <v>2921</v>
       </c>
       <c r="E20" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="205" t="s">
+        <v>3027</v>
+      </c>
+      <c r="B21" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C21" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D21" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -34129,6 +34607,7 @@
     <hyperlink ref="A15" r:id="rId17"/>
     <hyperlink ref="A17" r:id="rId18"/>
     <hyperlink ref="A18" r:id="rId19"/>
+    <hyperlink ref="A21" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34136,10 +34615,10 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:E67"/>
+      <selection activeCell="B68" sqref="B68:E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35259,7 +35738,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="205" t="s">
-        <v>2978</v>
+        <v>2977</v>
       </c>
       <c r="C67" s="215" t="s">
         <v>2920</v>
@@ -35268,6 +35747,23 @@
         <v>2921</v>
       </c>
       <c r="E67" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="206" t="s">
+        <v>3028</v>
+      </c>
+      <c r="B68" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C68" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D68" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E68" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -35338,6 +35834,7 @@
     <hyperlink ref="A63" r:id="rId63"/>
     <hyperlink ref="A64" r:id="rId64"/>
     <hyperlink ref="A65" r:id="rId65"/>
+    <hyperlink ref="A68" r:id="rId66"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -35345,10 +35842,10 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:E69"/>
+      <selection activeCell="B70" sqref="B70:E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36499,7 +36996,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="205" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="C69" s="215" t="s">
         <v>2920</v>
@@ -36508,6 +37005,23 @@
         <v>2921</v>
       </c>
       <c r="E69" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="206" t="s">
+        <v>3029</v>
+      </c>
+      <c r="B70" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C70" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D70" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -36580,6 +37094,7 @@
     <hyperlink ref="A65" r:id="rId65"/>
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
+    <hyperlink ref="A70" r:id="rId68"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -36587,10 +37102,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37898,7 +38413,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="182" t="s">
-        <v>2930</v>
+        <v>2929</v>
       </c>
       <c r="B78" s="215"/>
       <c r="C78" s="215" t="s">
@@ -37908,12 +38423,12 @@
         <v>2921</v>
       </c>
       <c r="E78" s="215" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="206" t="s">
-        <v>2931</v>
+        <v>2930</v>
       </c>
       <c r="B79" s="215" t="s">
         <v>2649</v>
@@ -37925,24 +38440,41 @@
         <v>21</v>
       </c>
       <c r="E79" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="206" t="s">
-        <v>2932</v>
+        <v>2931</v>
       </c>
       <c r="B80" s="215" t="s">
         <v>2649</v>
       </c>
       <c r="C80" s="215" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="D80" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E80" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="206" t="s">
+        <v>3003</v>
+      </c>
+      <c r="B81" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C81" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D81" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E81" s="217" t="s">
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -38021,6 +38553,7 @@
     <hyperlink ref="A71" r:id="rId72"/>
     <hyperlink ref="A79" r:id="rId73"/>
     <hyperlink ref="A80" r:id="rId74"/>
+    <hyperlink ref="A81" r:id="rId75"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -38028,10 +38561,10 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:E69"/>
+      <selection activeCell="B70" sqref="B70:E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39182,7 +39715,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="206" t="s">
-        <v>2980</v>
+        <v>2979</v>
       </c>
       <c r="C69" s="215" t="s">
         <v>2920</v>
@@ -39191,6 +39724,23 @@
         <v>2921</v>
       </c>
       <c r="E69" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="206" t="s">
+        <v>3030</v>
+      </c>
+      <c r="B70" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C70" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D70" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -39263,6 +39813,7 @@
     <hyperlink ref="A65" r:id="rId65"/>
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
+    <hyperlink ref="A70" r:id="rId68"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -39270,10 +39821,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:E66"/>
+      <selection activeCell="B67" sqref="B67:E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40381,7 +40932,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="206" t="s">
-        <v>2981</v>
+        <v>2980</v>
       </c>
       <c r="B66" s="215"/>
       <c r="C66" s="215" t="s">
@@ -40391,6 +40942,23 @@
         <v>2921</v>
       </c>
       <c r="E66" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="206" t="s">
+        <v>3031</v>
+      </c>
+      <c r="B67" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C67" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D67" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -40462,6 +41030,7 @@
     <hyperlink ref="A63" r:id="rId64"/>
     <hyperlink ref="A64" r:id="rId65"/>
     <hyperlink ref="A65" r:id="rId66"/>
+    <hyperlink ref="A67" r:id="rId67"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -40469,10 +41038,10 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64:E64"/>
+      <selection activeCell="B65" sqref="B65:E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41544,7 +42113,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="206" t="s">
-        <v>2982</v>
+        <v>2981</v>
       </c>
       <c r="C64" s="215" t="s">
         <v>2920</v>
@@ -41553,6 +42122,23 @@
         <v>2921</v>
       </c>
       <c r="E64" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="206" t="s">
+        <v>3032</v>
+      </c>
+      <c r="B65" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C65" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D65" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -41621,6 +42207,7 @@
     <hyperlink ref="A61" r:id="rId61"/>
     <hyperlink ref="A62" r:id="rId62"/>
     <hyperlink ref="A63" r:id="rId63"/>
+    <hyperlink ref="A65" r:id="rId64"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -41628,10 +42215,10 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:E19"/>
+      <selection activeCell="B20" sqref="B20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41944,7 +42531,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="206" t="s">
-        <v>2983</v>
+        <v>2982</v>
       </c>
       <c r="B19" s="215"/>
       <c r="C19" s="215" t="s">
@@ -41954,6 +42541,23 @@
         <v>2921</v>
       </c>
       <c r="E19" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="206" t="s">
+        <v>3033</v>
+      </c>
+      <c r="B20" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C20" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D20" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -41978,6 +42582,7 @@
     <hyperlink ref="A14" r:id="rId17"/>
     <hyperlink ref="A17" r:id="rId18"/>
     <hyperlink ref="A18" r:id="rId19"/>
+    <hyperlink ref="A20" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -41985,10 +42590,10 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:E68"/>
+      <selection activeCell="B69" sqref="B69:E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43130,7 +43735,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="215" t="s">
-        <v>2984</v>
+        <v>2983</v>
       </c>
       <c r="B68" s="215"/>
       <c r="C68" s="215" t="s">
@@ -43140,6 +43745,23 @@
         <v>2921</v>
       </c>
       <c r="E68" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="205" t="s">
+        <v>3034</v>
+      </c>
+      <c r="B69" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C69" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D69" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E69" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -43212,6 +43834,7 @@
     <hyperlink ref="A65" r:id="rId65"/>
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
+    <hyperlink ref="A69" r:id="rId68"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -43219,10 +43842,10 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:E19"/>
+      <selection activeCell="B20" sqref="B20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43535,7 +44158,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="206" t="s">
-        <v>2985</v>
+        <v>2984</v>
       </c>
       <c r="B19" s="215"/>
       <c r="C19" s="215" t="s">
@@ -43545,6 +44168,23 @@
         <v>2921</v>
       </c>
       <c r="E19" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="206" t="s">
+        <v>3035</v>
+      </c>
+      <c r="B20" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C20" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D20" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -43569,6 +44209,7 @@
     <hyperlink ref="A14" r:id="rId17"/>
     <hyperlink ref="A17" r:id="rId18"/>
     <hyperlink ref="A18" r:id="rId19"/>
+    <hyperlink ref="A20" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -43576,10 +44217,10 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:E20"/>
+      <selection activeCell="B21" sqref="B21:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43907,7 +44548,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="206" t="s">
-        <v>2986</v>
+        <v>2985</v>
       </c>
       <c r="B20" s="215"/>
       <c r="C20" s="215" t="s">
@@ -43917,6 +44558,23 @@
         <v>2921</v>
       </c>
       <c r="E20" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="206" t="s">
+        <v>3036</v>
+      </c>
+      <c r="B21" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C21" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D21" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -43942,6 +44600,7 @@
     <hyperlink ref="A17" r:id="rId18"/>
     <hyperlink ref="A18" r:id="rId19"/>
     <hyperlink ref="A19" r:id="rId20"/>
+    <hyperlink ref="A21" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -43949,10 +44608,10 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:E19"/>
+      <selection activeCell="B20" sqref="B20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44265,7 +44924,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="206" t="s">
-        <v>2987</v>
+        <v>2986</v>
       </c>
       <c r="B19" s="215"/>
       <c r="C19" s="215" t="s">
@@ -44275,6 +44934,23 @@
         <v>2921</v>
       </c>
       <c r="E19" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="206" t="s">
+        <v>3037</v>
+      </c>
+      <c r="B20" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C20" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D20" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -44299,6 +44975,7 @@
     <hyperlink ref="A14" r:id="rId17"/>
     <hyperlink ref="A17" r:id="rId18"/>
     <hyperlink ref="A18" r:id="rId19"/>
+    <hyperlink ref="A20" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -44306,10 +44983,10 @@
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:E69"/>
+      <selection activeCell="B70" sqref="B70:E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45468,7 +46145,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="206" t="s">
-        <v>2988</v>
+        <v>2987</v>
       </c>
       <c r="B69" s="215"/>
       <c r="C69" s="215" t="s">
@@ -45478,6 +46155,23 @@
         <v>2921</v>
       </c>
       <c r="E69" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="206" t="s">
+        <v>3038</v>
+      </c>
+      <c r="B70" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C70" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D70" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -45549,6 +46243,7 @@
     <hyperlink ref="A66" r:id="rId64"/>
     <hyperlink ref="A67" r:id="rId65"/>
     <hyperlink ref="A68" r:id="rId66"/>
+    <hyperlink ref="A70" r:id="rId67"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -45556,10 +46251,10 @@
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:E68"/>
+      <selection activeCell="B69" sqref="B69:E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46701,7 +47396,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="205" t="s">
-        <v>2989</v>
+        <v>2988</v>
       </c>
       <c r="B68" s="215"/>
       <c r="C68" s="215" t="s">
@@ -46711,6 +47406,23 @@
         <v>2921</v>
       </c>
       <c r="E68" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="206" t="s">
+        <v>3039</v>
+      </c>
+      <c r="B69" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C69" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D69" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E69" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -46784,6 +47496,7 @@
     <hyperlink ref="A65" r:id="rId66"/>
     <hyperlink ref="A66" r:id="rId67"/>
     <hyperlink ref="A67" r:id="rId68"/>
+    <hyperlink ref="A69" r:id="rId69"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -46791,10 +47504,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:E81"/>
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48119,7 +48832,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="181" t="s">
-        <v>2933</v>
+        <v>2932</v>
       </c>
       <c r="B79" s="215"/>
       <c r="C79" s="215" t="s">
@@ -48134,7 +48847,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="206" t="s">
-        <v>2934</v>
+        <v>2933</v>
       </c>
       <c r="B80" s="215" t="s">
         <v>2649</v>
@@ -48146,24 +48859,41 @@
         <v>21</v>
       </c>
       <c r="E80" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="206" t="s">
-        <v>2935</v>
+        <v>2934</v>
       </c>
       <c r="B81" s="215" t="s">
         <v>2649</v>
       </c>
       <c r="C81" s="215" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="D81" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E81" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="206" t="s">
+        <v>3004</v>
+      </c>
+      <c r="B82" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C82" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D82" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E82" s="217" t="s">
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -48241,6 +48971,7 @@
     <hyperlink ref="A71" r:id="rId71"/>
     <hyperlink ref="A80" r:id="rId72"/>
     <hyperlink ref="A81" r:id="rId73"/>
+    <hyperlink ref="A82" r:id="rId74"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -48248,10 +48979,10 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:E19"/>
+      <selection activeCell="B20" sqref="B20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48564,7 +49295,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="205" t="s">
-        <v>2990</v>
+        <v>2989</v>
       </c>
       <c r="B19" s="215"/>
       <c r="C19" s="215" t="s">
@@ -48574,6 +49305,23 @@
         <v>2921</v>
       </c>
       <c r="E19" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="206" t="s">
+        <v>3040</v>
+      </c>
+      <c r="B20" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C20" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D20" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -48598,6 +49346,7 @@
     <hyperlink ref="A16" r:id="rId17"/>
     <hyperlink ref="A17" r:id="rId18"/>
     <hyperlink ref="A18" r:id="rId19"/>
+    <hyperlink ref="A20" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -48605,10 +49354,10 @@
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:E70"/>
+      <selection activeCell="B71" sqref="B71:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49796,6 +50545,23 @@
         <v>0</v>
       </c>
       <c r="E70" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="206" t="s">
+        <v>3041</v>
+      </c>
+      <c r="B71" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C71" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D71" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -49871,6 +50637,7 @@
     <hyperlink ref="A68" r:id="rId68"/>
     <hyperlink ref="A69" r:id="rId69"/>
     <hyperlink ref="A70" r:id="rId70"/>
+    <hyperlink ref="A71" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -49878,10 +50645,10 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:E81"/>
+      <selection activeCell="B82" sqref="B82:E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51206,7 +51973,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="205" t="s">
-        <v>2991</v>
+        <v>2990</v>
       </c>
       <c r="B79" s="215"/>
       <c r="C79" s="215" t="s">
@@ -51221,7 +51988,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="206" t="s">
-        <v>2992</v>
+        <v>2991</v>
       </c>
       <c r="B80" s="215" t="s">
         <v>2649</v>
@@ -51233,24 +52000,41 @@
         <v>21</v>
       </c>
       <c r="E80" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="206" t="s">
-        <v>2993</v>
+        <v>2992</v>
       </c>
       <c r="B81" s="215" t="s">
         <v>2649</v>
       </c>
       <c r="C81" s="215" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="D81" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E81" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="206" t="s">
+        <v>3042</v>
+      </c>
+      <c r="B82" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C82" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D82" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E82" s="217" t="s">
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -51329,6 +52113,7 @@
     <hyperlink ref="A72" r:id="rId72"/>
     <hyperlink ref="A80" r:id="rId73"/>
     <hyperlink ref="A81" r:id="rId74"/>
+    <hyperlink ref="A82" r:id="rId75"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -51336,10 +52121,10 @@
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70:E70"/>
+      <selection activeCell="B71" sqref="B71:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52511,7 +53296,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="205" t="s">
-        <v>2994</v>
+        <v>2993</v>
       </c>
       <c r="B70" s="215"/>
       <c r="C70" s="215" t="s">
@@ -52521,6 +53306,23 @@
         <v>2921</v>
       </c>
       <c r="E70" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="206" t="s">
+        <v>3043</v>
+      </c>
+      <c r="B71" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C71" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D71" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -52594,6 +53396,7 @@
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
     <hyperlink ref="A68" r:id="rId68"/>
+    <hyperlink ref="A71" r:id="rId69"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -52601,10 +53404,10 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70:E70"/>
+      <selection activeCell="B71" sqref="B71:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53776,7 +54579,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="205" t="s">
-        <v>2995</v>
+        <v>2994</v>
       </c>
       <c r="B70" s="215"/>
       <c r="C70" s="215" t="s">
@@ -53786,6 +54589,23 @@
         <v>2921</v>
       </c>
       <c r="E70" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="206" t="s">
+        <v>3044</v>
+      </c>
+      <c r="B71" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C71" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D71" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -53859,6 +54679,7 @@
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
     <hyperlink ref="A68" r:id="rId68"/>
+    <hyperlink ref="A71" r:id="rId69"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -53866,10 +54687,10 @@
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:E66"/>
+      <selection activeCell="B67" sqref="B67:E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54977,7 +55798,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="175" t="s">
-        <v>2996</v>
+        <v>2995</v>
       </c>
       <c r="B66" s="215"/>
       <c r="C66" s="215" t="s">
@@ -54987,6 +55808,23 @@
         <v>2921</v>
       </c>
       <c r="E66" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="206" t="s">
+        <v>3045</v>
+      </c>
+      <c r="B67" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C67" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D67" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -55058,6 +55896,7 @@
     <hyperlink ref="A64" r:id="rId64"/>
     <hyperlink ref="A65" r:id="rId65"/>
     <hyperlink ref="A66" r:id="rId66"/>
+    <hyperlink ref="A67" r:id="rId67"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -55065,10 +55904,10 @@
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:E66"/>
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56176,7 +57015,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="206" t="s">
-        <v>2997</v>
+        <v>2996</v>
       </c>
       <c r="B66" s="215"/>
       <c r="C66" s="215" t="s">
@@ -56186,6 +57025,23 @@
         <v>2921</v>
       </c>
       <c r="E66" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="206" t="s">
+        <v>3046</v>
+      </c>
+      <c r="B67" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C67" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D67" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -56256,6 +57112,7 @@
     <hyperlink ref="A63" r:id="rId63"/>
     <hyperlink ref="A64" r:id="rId64"/>
     <hyperlink ref="A65" r:id="rId65"/>
+    <hyperlink ref="A67" r:id="rId66"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -56266,7 +57123,7 @@
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:E27"/>
+      <selection activeCell="B28" sqref="B28:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56707,7 +57564,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="205" t="s">
-        <v>2998</v>
+        <v>2997</v>
       </c>
       <c r="B27" s="215"/>
       <c r="C27" s="215" t="s">
@@ -56717,6 +57574,23 @@
         <v>2921</v>
       </c>
       <c r="E27" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="206" t="s">
+        <v>3047</v>
+      </c>
+      <c r="B28" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C28" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D28" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -56804,6 +57678,7 @@
     <hyperlink ref="A23" r:id="rId24"/>
     <hyperlink ref="A24" r:id="rId25"/>
     <hyperlink ref="A25" r:id="rId26"/>
+    <hyperlink ref="A28" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -56811,10 +57686,10 @@
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57922,7 +58797,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
-        <v>2999</v>
+        <v>2998</v>
       </c>
       <c r="B66" s="215"/>
       <c r="C66" s="215" t="s">
@@ -57932,6 +58807,23 @@
         <v>2921</v>
       </c>
       <c r="E66" s="215" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="206" t="s">
+        <v>3048</v>
+      </c>
+      <c r="B67" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C67" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D67" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" s="217" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -58003,6 +58895,7 @@
     <hyperlink ref="A64" r:id="rId64"/>
     <hyperlink ref="A65" r:id="rId65"/>
     <hyperlink ref="A66" r:id="rId66"/>
+    <hyperlink ref="A67" r:id="rId67"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -58010,10 +58903,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:E80"/>
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59318,7 +60211,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="182" t="s">
-        <v>2936</v>
+        <v>2935</v>
       </c>
       <c r="B78" s="215"/>
       <c r="C78" s="215" t="s">
@@ -59328,12 +60221,12 @@
         <v>2921</v>
       </c>
       <c r="E78" s="215" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="206" t="s">
-        <v>2937</v>
+        <v>2936</v>
       </c>
       <c r="B79" s="215" t="s">
         <v>2649</v>
@@ -59345,24 +60238,41 @@
         <v>21</v>
       </c>
       <c r="E79" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="206" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="B80" s="215" t="s">
         <v>2649</v>
       </c>
       <c r="C80" s="215" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="D80" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E80" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="206" t="s">
+        <v>3005</v>
+      </c>
+      <c r="B81" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C81" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D81" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E81" s="217" t="s">
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -59439,6 +60349,7 @@
     <hyperlink ref="A70" r:id="rId70"/>
     <hyperlink ref="A79" r:id="rId71"/>
     <hyperlink ref="A80" r:id="rId72"/>
+    <hyperlink ref="A81" r:id="rId73"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -59446,10 +60357,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60023,7 +60934,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
-        <v>3000</v>
+        <v>2999</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>26</v>
@@ -60792,7 +61703,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="205" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="B80" s="215"/>
       <c r="C80" s="215" t="s">
@@ -60807,7 +61718,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="206" t="s">
-        <v>2940</v>
+        <v>2939</v>
       </c>
       <c r="B81" s="215" t="s">
         <v>2649</v>
@@ -60819,24 +61730,41 @@
         <v>21</v>
       </c>
       <c r="E81" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="206" t="s">
-        <v>2941</v>
+        <v>2940</v>
       </c>
       <c r="B82" s="215" t="s">
         <v>2649</v>
       </c>
       <c r="C82" s="215" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="D82" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E82" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="206" t="s">
+        <v>3006</v>
+      </c>
+      <c r="B83" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C83" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D83" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="217" t="s">
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -60918,18 +61846,19 @@
     <hyperlink ref="A35" r:id="rId75"/>
     <hyperlink ref="A33" r:id="rId76"/>
     <hyperlink ref="A34" r:id="rId77"/>
+    <hyperlink ref="A83" r:id="rId78"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId78"/>
+  <pageSetup orientation="portrait" r:id="rId79"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:E81"/>
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62255,7 +63184,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="181" t="s">
-        <v>2942</v>
+        <v>2941</v>
       </c>
       <c r="B79" s="215"/>
       <c r="C79" s="215" t="s">
@@ -62270,7 +63199,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="206" t="s">
-        <v>2943</v>
+        <v>2942</v>
       </c>
       <c r="B80" s="215" t="s">
         <v>2649</v>
@@ -62282,24 +63211,41 @@
         <v>21</v>
       </c>
       <c r="E80" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="206" t="s">
-        <v>2944</v>
+        <v>2943</v>
       </c>
       <c r="B81" s="215" t="s">
         <v>2649</v>
       </c>
       <c r="C81" s="215" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="D81" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E81" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="206" t="s">
+        <v>3007</v>
+      </c>
+      <c r="B82" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C82" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D82" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E82" s="217" t="s">
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -62379,6 +63325,7 @@
     <hyperlink ref="A71" r:id="rId73"/>
     <hyperlink ref="A80" r:id="rId74"/>
     <hyperlink ref="A81" r:id="rId75"/>
+    <hyperlink ref="A82" r:id="rId76"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -62386,10 +63333,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:E80"/>
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63698,7 +64645,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="205" t="s">
-        <v>2945</v>
+        <v>2944</v>
       </c>
       <c r="B78" s="215"/>
       <c r="C78" s="215" t="s">
@@ -63713,7 +64660,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="199" t="s">
-        <v>2946</v>
+        <v>2945</v>
       </c>
       <c r="B79" s="215" t="s">
         <v>2649</v>
@@ -63725,24 +64672,41 @@
         <v>21</v>
       </c>
       <c r="E79" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="206" t="s">
-        <v>2947</v>
+        <v>2946</v>
       </c>
       <c r="B80" s="215" t="s">
         <v>2649</v>
       </c>
       <c r="C80" s="215" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="D80" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E80" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="199" t="s">
+        <v>3008</v>
+      </c>
+      <c r="B81" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C81" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D81" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E81" s="217" t="s">
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -63818,18 +64782,19 @@
     <hyperlink ref="A70" r:id="rId69"/>
     <hyperlink ref="A78" r:id="rId70"/>
     <hyperlink ref="A80" r:id="rId71"/>
+    <hyperlink ref="A81" r:id="rId72"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId72"/>
+  <pageSetup orientation="portrait" r:id="rId73"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:E81"/>
+      <selection activeCell="B82" sqref="B82:E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -65155,7 +66120,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="215" t="s">
-        <v>2948</v>
+        <v>2947</v>
       </c>
       <c r="B79" s="215"/>
       <c r="C79" s="215" t="s">
@@ -65170,7 +66135,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="206" t="s">
-        <v>2949</v>
+        <v>2948</v>
       </c>
       <c r="B80" s="215" t="s">
         <v>2649</v>
@@ -65182,24 +66147,41 @@
         <v>21</v>
       </c>
       <c r="E80" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="206" t="s">
-        <v>2950</v>
+        <v>2949</v>
       </c>
       <c r="B81" s="215" t="s">
         <v>2649</v>
       </c>
       <c r="C81" s="215" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="D81" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E81" s="217" t="s">
-        <v>2924</v>
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="215" t="s">
+        <v>3009</v>
+      </c>
+      <c r="B82" s="215" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C82" s="215" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D82" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E82" s="217" t="s">
+        <v>2075</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added webvar7 6th url
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
+++ b/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdevalka\OVW Migration Project\Daily Checkout\13 Jan\Evening\OVWMigration\docs\OVW Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_OVWMig\jan_13\OVWMigration\docs\OVW Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11010" firstSheet="34" activeTab="41"/>
   </bookViews>
   <sheets>
     <sheet name="ja_jp" sheetId="48" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15274" uniqueCount="3049">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15349" uniqueCount="3065">
   <si>
     <t>products</t>
   </si>
@@ -9218,6 +9218,54 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/BE/fr/midsize/products_solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/solution/trends/iot/iot-products.html</t>
+  </si>
+  <si>
+    <t>iot-products-webvar7</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CN/solutions/trends/iot/iot-products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/cisco/web/UK/solutions/trends/iot/iot-products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/solutions/trends/iot/iot-products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/LA/soluciones/trends/iot/iot-products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/solucoes/trends/iot/iot-products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/ar/solutions/trends/iot/iot-products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/solutions/trends/iot/iot-products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FR/solutions/trends/iot/iot-products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/solutions/trends/iot/iot-products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/solutions/trends/iot/iot-products_fr.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IN/solutions/trends/iot/iot-products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ANZ/netsol/trends/iot/iot-products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/KR/networking/trends/iot/iot-products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/solutions/trends/iot/iot-products.html</t>
   </si>
 </sst>
 </file>
@@ -9979,10 +10027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79:E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11300,6 +11348,23 @@
         <v>21</v>
       </c>
       <c r="E78" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="215" t="s">
+        <v>3049</v>
+      </c>
+      <c r="B79" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C79" s="215" t="s">
+        <v>3050</v>
+      </c>
+      <c r="D79" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E79" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -11383,10 +11448,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
     <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81:E81"/>
+      <selection activeCell="A82" sqref="A82:E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12756,6 +12821,23 @@
         <v>21</v>
       </c>
       <c r="E81" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="215" t="s">
+        <v>3059</v>
+      </c>
+      <c r="B82" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C82" s="215" t="s">
+        <v>3050</v>
+      </c>
+      <c r="D82" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E82" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -12843,10 +12925,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82:E82"/>
+      <selection activeCell="A83" sqref="A83:E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14232,6 +14314,23 @@
         <v>21</v>
       </c>
       <c r="E82" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="215" t="s">
+        <v>3060</v>
+      </c>
+      <c r="B83" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C83" s="215" t="s">
+        <v>3050</v>
+      </c>
+      <c r="D83" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -14320,10 +14419,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81:E81"/>
+      <selection activeCell="A82" sqref="A82:E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15689,6 +15788,23 @@
         <v>21</v>
       </c>
       <c r="E81" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="215" t="s">
+        <v>3062</v>
+      </c>
+      <c r="B82" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C82" s="215" t="s">
+        <v>3050</v>
+      </c>
+      <c r="D82" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E82" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -15774,10 +15890,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83:E83"/>
+      <selection activeCell="A84" sqref="A84:E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17180,6 +17296,23 @@
         <v>21</v>
       </c>
       <c r="E83" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="215" t="s">
+        <v>3061</v>
+      </c>
+      <c r="B84" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C84" s="215" t="s">
+        <v>3050</v>
+      </c>
+      <c r="D84" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -17270,10 +17403,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83:E83"/>
+      <selection activeCell="A84" sqref="A84:E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18676,6 +18809,23 @@
         <v>21</v>
       </c>
       <c r="E83" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="215" t="s">
+        <v>3063</v>
+      </c>
+      <c r="B84" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C84" s="215" t="s">
+        <v>3050</v>
+      </c>
+      <c r="D84" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -24270,10 +24420,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:E77"/>
+      <selection activeCell="A78" sqref="A78:E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25575,6 +25725,23 @@
         <v>21</v>
       </c>
       <c r="E77" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="215" t="s">
+        <v>3051</v>
+      </c>
+      <c r="B78" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C78" s="215" t="s">
+        <v>3050</v>
+      </c>
+      <c r="D78" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -37102,10 +37269,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+      <selection activeCell="A82" sqref="A82:E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38474,6 +38641,23 @@
         <v>21</v>
       </c>
       <c r="E81" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="215" t="s">
+        <v>3052</v>
+      </c>
+      <c r="B82" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C82" s="215" t="s">
+        <v>3050</v>
+      </c>
+      <c r="D82" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E82" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -47504,10 +47688,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+      <selection activeCell="A83" sqref="A83:E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48893,6 +49077,23 @@
         <v>21</v>
       </c>
       <c r="E82" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="215" t="s">
+        <v>3053</v>
+      </c>
+      <c r="B83" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C83" s="215" t="s">
+        <v>3050</v>
+      </c>
+      <c r="D83" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -50645,10 +50846,10 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82:E82"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83:E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52034,6 +52235,23 @@
         <v>21</v>
       </c>
       <c r="E82" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="215" t="s">
+        <v>3064</v>
+      </c>
+      <c r="B83" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C83" s="215" t="s">
+        <v>3050</v>
+      </c>
+      <c r="D83" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -58903,10 +59121,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+      <selection activeCell="A82" sqref="A82:E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60272,6 +60490,23 @@
         <v>21</v>
       </c>
       <c r="E81" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="215" t="s">
+        <v>3054</v>
+      </c>
+      <c r="B82" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C82" s="215" t="s">
+        <v>3050</v>
+      </c>
+      <c r="D82" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E82" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -60357,10 +60592,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+      <selection activeCell="A84" sqref="A84:E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61764,6 +61999,23 @@
         <v>21</v>
       </c>
       <c r="E83" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="215" t="s">
+        <v>3055</v>
+      </c>
+      <c r="B84" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C84" s="215" t="s">
+        <v>3050</v>
+      </c>
+      <c r="D84" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -61855,10 +62107,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83"/>
+      <selection activeCell="A83" sqref="A83:E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63245,6 +63497,23 @@
         <v>21</v>
       </c>
       <c r="E82" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="215" t="s">
+        <v>3056</v>
+      </c>
+      <c r="B83" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C83" s="215" t="s">
+        <v>3050</v>
+      </c>
+      <c r="D83" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -63333,10 +63602,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+      <selection activeCell="A82" sqref="A82:E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64706,6 +64975,23 @@
         <v>21</v>
       </c>
       <c r="E81" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="215" t="s">
+        <v>3057</v>
+      </c>
+      <c r="B82" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C82" s="215" t="s">
+        <v>3050</v>
+      </c>
+      <c r="D82" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E82" s="215" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -64791,10 +65077,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82:E82"/>
+      <selection activeCell="A83" sqref="A83:E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -66181,6 +66467,23 @@
         <v>21</v>
       </c>
       <c r="E82" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="215" t="s">
+        <v>3058</v>
+      </c>
+      <c r="B83" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C83" s="215" t="s">
+        <v>3050</v>
+      </c>
+      <c r="D83" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="215" t="s">
         <v>2075</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated the OVW all url excel
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
+++ b/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_OVWMig\jan_13\OVWMigration\docs\OVW Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW-jan14\OVWMigration\docs\OVW Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15349" uniqueCount="3065">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15499" uniqueCount="3098">
   <si>
     <t>products</t>
   </si>
@@ -9266,6 +9266,105 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/ME/solutions/trends/iot/iot-products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/solution/trends/iot/iot_services.html</t>
+  </si>
+  <si>
+    <t>services-iotproductsvar12</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/solution/trends/iot/solutions.html</t>
+  </si>
+  <si>
+    <t>solutions-iotproductsvar12</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CN/solutions/trends/iot/iot_services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CN/solutions/trends/iot/solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/cisco/web/UK/solutions/trends/iot/iot_services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/cisco/web/UK/solutions/trends/iot/solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/solutions/trends/iot/iot_services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/solutions/trends/iot/solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/LA/soluciones/trends/iot/iot_services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/LA/soluciones/trends/iot/solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/solucoes/trends/iot/iot_services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/solucoes/trends/iot/solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/ar/solutions/trends/iot/iot_services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/ar/solutions/trends/iot/solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/solutions/trends/iot/iot_services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/solutions/trends/iot/solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FR/solutions/trends/iot/iot_services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FR/solutions/trends/iot/solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ANZ/netsol/trends/iot/iot_services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/solutions/trends/iot/iot_services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/solutions/trends/iot/iot_services_fr.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IN/solutions/trends/iot/iot_services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/KR/networking/trends/iot/iot_services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/solutions/trends/iot/iot_services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ANZ/netsol/trends/iot/solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/solutions/trends/iot/solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/solutions/trends/iot/solutions_fr.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IN/solutions/trends/iot/solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/KR/networking/trends/iot/solutions.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/solutions/trends/iot/solutions.html</t>
   </si>
 </sst>
 </file>
@@ -10027,10 +10126,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:E79"/>
+      <selection activeCell="B81" sqref="B81:E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11366,6 +11465,40 @@
       </c>
       <c r="E79" s="215" t="s">
         <v>2075</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="19" t="s">
+        <v>3065</v>
+      </c>
+      <c r="B80" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C80" s="215" t="s">
+        <v>3066</v>
+      </c>
+      <c r="D80" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E80" s="217" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="19" t="s">
+        <v>3068</v>
+      </c>
+      <c r="B81" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C81" s="215" t="s">
+        <v>3069</v>
+      </c>
+      <c r="D81" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E81" s="217" t="s">
+        <v>3067</v>
       </c>
     </row>
   </sheetData>
@@ -11440,18 +11573,20 @@
     <hyperlink ref="A67" r:id="rId68"/>
     <hyperlink ref="A76" r:id="rId69"/>
     <hyperlink ref="A77" r:id="rId70"/>
+    <hyperlink ref="A80" r:id="rId71"/>
+    <hyperlink ref="A81" r:id="rId72"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId71"/>
+  <pageSetup orientation="portrait" r:id="rId73"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82:E82"/>
+      <selection activeCell="B84" sqref="B84:E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12839,6 +12974,40 @@
       </c>
       <c r="E82" s="215" t="s">
         <v>2075</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="206" t="s">
+        <v>3087</v>
+      </c>
+      <c r="B83" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C83" s="215" t="s">
+        <v>3066</v>
+      </c>
+      <c r="D83" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="217" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="206" t="s">
+        <v>3093</v>
+      </c>
+      <c r="B84" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C84" s="215" t="s">
+        <v>3069</v>
+      </c>
+      <c r="D84" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="217" t="s">
+        <v>3067</v>
       </c>
     </row>
   </sheetData>
@@ -12918,6 +13087,8 @@
     <hyperlink ref="A79" r:id="rId73"/>
     <hyperlink ref="A80" r:id="rId74"/>
     <hyperlink ref="A81" r:id="rId75"/>
+    <hyperlink ref="A83" r:id="rId76"/>
+    <hyperlink ref="A84" r:id="rId77"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12925,10 +13096,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83:E83"/>
+      <selection activeCell="B85" sqref="B85:E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14332,6 +14503,40 @@
       </c>
       <c r="E83" s="215" t="s">
         <v>2075</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="206" t="s">
+        <v>3088</v>
+      </c>
+      <c r="B84" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C84" s="215" t="s">
+        <v>3066</v>
+      </c>
+      <c r="D84" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="217" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="206" t="s">
+        <v>3094</v>
+      </c>
+      <c r="B85" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C85" s="215" t="s">
+        <v>3069</v>
+      </c>
+      <c r="D85" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E85" s="217" t="s">
+        <v>3067</v>
       </c>
     </row>
   </sheetData>
@@ -14412,6 +14617,8 @@
     <hyperlink ref="A80" r:id="rId74"/>
     <hyperlink ref="A81" r:id="rId75"/>
     <hyperlink ref="A82" r:id="rId76"/>
+    <hyperlink ref="A84" r:id="rId77"/>
+    <hyperlink ref="A85" r:id="rId78"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14419,10 +14626,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82:E82"/>
+      <selection activeCell="B84" sqref="B84:E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15806,6 +16013,40 @@
       </c>
       <c r="E82" s="215" t="s">
         <v>2075</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="206" t="s">
+        <v>3086</v>
+      </c>
+      <c r="B83" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C83" s="215" t="s">
+        <v>3066</v>
+      </c>
+      <c r="D83" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="217" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="206" t="s">
+        <v>3092</v>
+      </c>
+      <c r="B84" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C84" s="215" t="s">
+        <v>3069</v>
+      </c>
+      <c r="D84" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="217" t="s">
+        <v>3067</v>
       </c>
     </row>
   </sheetData>
@@ -15883,6 +16124,8 @@
     <hyperlink ref="A79" r:id="rId71"/>
     <hyperlink ref="A80" r:id="rId72"/>
     <hyperlink ref="A81" r:id="rId73"/>
+    <hyperlink ref="A83" r:id="rId74"/>
+    <hyperlink ref="A84" r:id="rId75"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15890,10 +16133,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84:E84"/>
+      <selection activeCell="B86" sqref="B86:E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17314,6 +17557,40 @@
       </c>
       <c r="E84" s="215" t="s">
         <v>2075</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="206" t="s">
+        <v>3089</v>
+      </c>
+      <c r="B85" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C85" s="215" t="s">
+        <v>3066</v>
+      </c>
+      <c r="D85" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E85" s="217" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="206" t="s">
+        <v>3095</v>
+      </c>
+      <c r="B86" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C86" s="215" t="s">
+        <v>3069</v>
+      </c>
+      <c r="D86" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E86" s="217" t="s">
+        <v>3067</v>
       </c>
     </row>
   </sheetData>
@@ -17395,18 +17672,20 @@
     <hyperlink ref="A82" r:id="rId75"/>
     <hyperlink ref="A80" r:id="rId76"/>
     <hyperlink ref="A83" r:id="rId77"/>
+    <hyperlink ref="A85" r:id="rId78"/>
+    <hyperlink ref="A86" r:id="rId79"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId78"/>
+  <pageSetup orientation="portrait" r:id="rId80"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84:E84"/>
+      <selection activeCell="B86" sqref="B86:E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18827,6 +19106,40 @@
       </c>
       <c r="E84" s="215" t="s">
         <v>2075</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="205" t="s">
+        <v>3090</v>
+      </c>
+      <c r="B85" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C85" s="215" t="s">
+        <v>3066</v>
+      </c>
+      <c r="D85" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E85" s="217" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="205" t="s">
+        <v>3096</v>
+      </c>
+      <c r="B86" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C86" s="215" t="s">
+        <v>3069</v>
+      </c>
+      <c r="D86" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E86" s="217" t="s">
+        <v>3067</v>
       </c>
     </row>
   </sheetData>
@@ -18907,6 +19220,8 @@
     <hyperlink ref="A81" r:id="rId74"/>
     <hyperlink ref="A82" r:id="rId75"/>
     <hyperlink ref="A83" r:id="rId76"/>
+    <hyperlink ref="A85" r:id="rId77"/>
+    <hyperlink ref="A86" r:id="rId78"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24420,10 +24735,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:E78"/>
+      <selection activeCell="A79" sqref="A79:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25743,6 +26058,40 @@
       </c>
       <c r="E78" s="215" t="s">
         <v>2075</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="19" t="s">
+        <v>3070</v>
+      </c>
+      <c r="B79" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C79" s="215" t="s">
+        <v>3066</v>
+      </c>
+      <c r="D79" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E79" s="217" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="19" t="s">
+        <v>3071</v>
+      </c>
+      <c r="B80" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C80" s="215" t="s">
+        <v>3069</v>
+      </c>
+      <c r="D80" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E80" s="217" t="s">
+        <v>3067</v>
       </c>
     </row>
   </sheetData>
@@ -25817,6 +26166,8 @@
     <hyperlink ref="A68" r:id="rId68"/>
     <hyperlink ref="A76" r:id="rId69"/>
     <hyperlink ref="A77" r:id="rId70"/>
+    <hyperlink ref="A79" r:id="rId71"/>
+    <hyperlink ref="A80" r:id="rId72"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -37269,10 +37620,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82:E82"/>
+      <selection activeCell="B83" sqref="B83:E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38659,6 +39010,40 @@
       </c>
       <c r="E82" s="215" t="s">
         <v>2075</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="19" t="s">
+        <v>3072</v>
+      </c>
+      <c r="B83" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C83" s="215" t="s">
+        <v>3066</v>
+      </c>
+      <c r="D83" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="217" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="19" t="s">
+        <v>3073</v>
+      </c>
+      <c r="B84" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C84" s="215" t="s">
+        <v>3069</v>
+      </c>
+      <c r="D84" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="217" t="s">
+        <v>3067</v>
       </c>
     </row>
   </sheetData>
@@ -38738,6 +39123,8 @@
     <hyperlink ref="A79" r:id="rId73"/>
     <hyperlink ref="A80" r:id="rId74"/>
     <hyperlink ref="A81" r:id="rId75"/>
+    <hyperlink ref="A83" r:id="rId76"/>
+    <hyperlink ref="A84" r:id="rId77"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -47688,10 +48075,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83:E83"/>
+      <selection activeCell="A84" sqref="A84:XFD85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49095,6 +49482,40 @@
       </c>
       <c r="E83" s="215" t="s">
         <v>2075</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="19" t="s">
+        <v>3074</v>
+      </c>
+      <c r="B84" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C84" s="215" t="s">
+        <v>3066</v>
+      </c>
+      <c r="D84" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="217" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="19" t="s">
+        <v>3075</v>
+      </c>
+      <c r="B85" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C85" s="215" t="s">
+        <v>3069</v>
+      </c>
+      <c r="D85" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E85" s="217" t="s">
+        <v>3067</v>
       </c>
     </row>
   </sheetData>
@@ -49173,6 +49594,8 @@
     <hyperlink ref="A80" r:id="rId72"/>
     <hyperlink ref="A81" r:id="rId73"/>
     <hyperlink ref="A82" r:id="rId74"/>
+    <hyperlink ref="A84" r:id="rId75"/>
+    <hyperlink ref="A85" r:id="rId76"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -50846,10 +51269,10 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83:E83"/>
+      <selection activeCell="B85" sqref="B85:E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52253,6 +52676,40 @@
       </c>
       <c r="E83" s="215" t="s">
         <v>2075</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="206" t="s">
+        <v>3091</v>
+      </c>
+      <c r="B84" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C84" s="215" t="s">
+        <v>3066</v>
+      </c>
+      <c r="D84" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="217" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="206" t="s">
+        <v>3097</v>
+      </c>
+      <c r="B85" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C85" s="215" t="s">
+        <v>3069</v>
+      </c>
+      <c r="D85" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E85" s="217" t="s">
+        <v>3067</v>
       </c>
     </row>
   </sheetData>
@@ -52332,6 +52789,8 @@
     <hyperlink ref="A80" r:id="rId73"/>
     <hyperlink ref="A81" r:id="rId74"/>
     <hyperlink ref="A82" r:id="rId75"/>
+    <hyperlink ref="A84" r:id="rId76"/>
+    <hyperlink ref="A85" r:id="rId77"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -59121,10 +59580,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82:E82"/>
+      <selection activeCell="A83" sqref="A83:XFD84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60508,6 +60967,40 @@
       </c>
       <c r="E82" s="215" t="s">
         <v>2075</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="19" t="s">
+        <v>3076</v>
+      </c>
+      <c r="B83" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C83" s="215" t="s">
+        <v>3066</v>
+      </c>
+      <c r="D83" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="217" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="19" t="s">
+        <v>3077</v>
+      </c>
+      <c r="B84" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C84" s="215" t="s">
+        <v>3069</v>
+      </c>
+      <c r="D84" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="217" t="s">
+        <v>3067</v>
       </c>
     </row>
   </sheetData>
@@ -60585,6 +61078,8 @@
     <hyperlink ref="A79" r:id="rId71"/>
     <hyperlink ref="A80" r:id="rId72"/>
     <hyperlink ref="A81" r:id="rId73"/>
+    <hyperlink ref="A83" r:id="rId74"/>
+    <hyperlink ref="A84" r:id="rId75"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -60592,10 +61087,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84:E84"/>
+      <selection activeCell="A85" sqref="A85:XFD86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62017,6 +62512,40 @@
       </c>
       <c r="E84" s="215" t="s">
         <v>2075</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="19" t="s">
+        <v>3078</v>
+      </c>
+      <c r="B85" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C85" s="215" t="s">
+        <v>3066</v>
+      </c>
+      <c r="D85" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E85" s="217" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="19" t="s">
+        <v>3079</v>
+      </c>
+      <c r="B86" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C86" s="215" t="s">
+        <v>3069</v>
+      </c>
+      <c r="D86" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E86" s="217" t="s">
+        <v>3067</v>
       </c>
     </row>
   </sheetData>
@@ -62099,18 +62628,20 @@
     <hyperlink ref="A33" r:id="rId76"/>
     <hyperlink ref="A34" r:id="rId77"/>
     <hyperlink ref="A83" r:id="rId78"/>
+    <hyperlink ref="A85" r:id="rId79"/>
+    <hyperlink ref="A86" r:id="rId80"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId79"/>
+  <pageSetup orientation="portrait" r:id="rId81"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83:E83"/>
+      <selection activeCell="A84" sqref="A84:XFD85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63515,6 +64046,40 @@
       </c>
       <c r="E83" s="215" t="s">
         <v>2075</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="19" t="s">
+        <v>3080</v>
+      </c>
+      <c r="B84" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C84" s="215" t="s">
+        <v>3066</v>
+      </c>
+      <c r="D84" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="217" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="19" t="s">
+        <v>3081</v>
+      </c>
+      <c r="B85" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C85" s="215" t="s">
+        <v>3069</v>
+      </c>
+      <c r="D85" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E85" s="217" t="s">
+        <v>3067</v>
       </c>
     </row>
   </sheetData>
@@ -63595,6 +64160,8 @@
     <hyperlink ref="A80" r:id="rId74"/>
     <hyperlink ref="A81" r:id="rId75"/>
     <hyperlink ref="A82" r:id="rId76"/>
+    <hyperlink ref="A84" r:id="rId77"/>
+    <hyperlink ref="A85" r:id="rId78"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -63602,10 +64169,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82:E82"/>
+      <selection activeCell="A83" sqref="A83:XFD84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64993,6 +65560,40 @@
       </c>
       <c r="E82" s="215" t="s">
         <v>2075</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="19" t="s">
+        <v>3082</v>
+      </c>
+      <c r="B83" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C83" s="215" t="s">
+        <v>3066</v>
+      </c>
+      <c r="D83" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="217" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="19" t="s">
+        <v>3083</v>
+      </c>
+      <c r="B84" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C84" s="215" t="s">
+        <v>3069</v>
+      </c>
+      <c r="D84" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="217" t="s">
+        <v>3067</v>
       </c>
     </row>
   </sheetData>
@@ -65069,18 +65670,20 @@
     <hyperlink ref="A78" r:id="rId70"/>
     <hyperlink ref="A80" r:id="rId71"/>
     <hyperlink ref="A81" r:id="rId72"/>
+    <hyperlink ref="A83" r:id="rId73"/>
+    <hyperlink ref="A84" r:id="rId74"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId73"/>
+  <pageSetup orientation="portrait" r:id="rId75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83:E83"/>
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -66485,6 +67088,40 @@
       </c>
       <c r="E83" s="215" t="s">
         <v>2075</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="19" t="s">
+        <v>3084</v>
+      </c>
+      <c r="B84" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C84" s="215" t="s">
+        <v>3066</v>
+      </c>
+      <c r="D84" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="217" t="s">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="19" t="s">
+        <v>3085</v>
+      </c>
+      <c r="B85" s="215" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C85" s="215" t="s">
+        <v>3069</v>
+      </c>
+      <c r="D85" s="215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E85" s="217" t="s">
+        <v>3067</v>
       </c>
     </row>
   </sheetData>
@@ -66562,6 +67199,8 @@
     <hyperlink ref="A71" r:id="rId71"/>
     <hyperlink ref="A80" r:id="rId72"/>
     <hyperlink ref="A81" r:id="rId73"/>
+    <hyperlink ref="A84" r:id="rId74"/>
+    <hyperlink ref="A85" r:id="rId75"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated ovw 48 url excel
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
+++ b/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15499" uniqueCount="3098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15499" uniqueCount="3097">
   <si>
     <t>products</t>
   </si>
@@ -9272,9 +9272,6 @@
   </si>
   <si>
     <t>services-iotproductsvar12</t>
-  </si>
-  <si>
-    <t>YES</t>
   </si>
   <si>
     <t>http://www.cisco.com/web/JP/solution/trends/iot/solutions.html</t>
@@ -11481,24 +11478,24 @@
         <v>21</v>
       </c>
       <c r="E80" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="19" t="s">
-        <v>3068</v>
+        <v>3067</v>
       </c>
       <c r="B81" s="215" t="s">
         <v>2708</v>
       </c>
       <c r="C81" s="215" t="s">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D81" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E81" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -12978,7 +12975,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="206" t="s">
-        <v>3087</v>
+        <v>3086</v>
       </c>
       <c r="B83" s="215" t="s">
         <v>2708</v>
@@ -12990,24 +12987,24 @@
         <v>21</v>
       </c>
       <c r="E83" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="206" t="s">
-        <v>3093</v>
+        <v>3092</v>
       </c>
       <c r="B84" s="215" t="s">
         <v>2708</v>
       </c>
       <c r="C84" s="215" t="s">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D84" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E84" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -14507,7 +14504,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="206" t="s">
-        <v>3088</v>
+        <v>3087</v>
       </c>
       <c r="B84" s="215" t="s">
         <v>2708</v>
@@ -14519,24 +14516,24 @@
         <v>21</v>
       </c>
       <c r="E84" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="206" t="s">
-        <v>3094</v>
+        <v>3093</v>
       </c>
       <c r="B85" s="215" t="s">
         <v>2708</v>
       </c>
       <c r="C85" s="215" t="s">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D85" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E85" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -16017,7 +16014,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="206" t="s">
-        <v>3086</v>
+        <v>3085</v>
       </c>
       <c r="B83" s="215" t="s">
         <v>2708</v>
@@ -16029,24 +16026,24 @@
         <v>21</v>
       </c>
       <c r="E83" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="206" t="s">
-        <v>3092</v>
+        <v>3091</v>
       </c>
       <c r="B84" s="215" t="s">
         <v>2708</v>
       </c>
       <c r="C84" s="215" t="s">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D84" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E84" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -17561,7 +17558,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="206" t="s">
-        <v>3089</v>
+        <v>3088</v>
       </c>
       <c r="B85" s="215" t="s">
         <v>2708</v>
@@ -17573,24 +17570,24 @@
         <v>21</v>
       </c>
       <c r="E85" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="206" t="s">
-        <v>3095</v>
+        <v>3094</v>
       </c>
       <c r="B86" s="215" t="s">
         <v>2708</v>
       </c>
       <c r="C86" s="215" t="s">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D86" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E86" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -19110,7 +19107,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="205" t="s">
-        <v>3090</v>
+        <v>3089</v>
       </c>
       <c r="B85" s="215" t="s">
         <v>2708</v>
@@ -19122,24 +19119,24 @@
         <v>21</v>
       </c>
       <c r="E85" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="205" t="s">
-        <v>3096</v>
+        <v>3095</v>
       </c>
       <c r="B86" s="215" t="s">
         <v>2708</v>
       </c>
       <c r="C86" s="215" t="s">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D86" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E86" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -26062,7 +26059,7 @@
     </row>
     <row r="79" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="19" t="s">
-        <v>3070</v>
+        <v>3069</v>
       </c>
       <c r="B79" s="215" t="s">
         <v>2708</v>
@@ -26074,24 +26071,24 @@
         <v>21</v>
       </c>
       <c r="E79" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="19" t="s">
-        <v>3071</v>
+        <v>3070</v>
       </c>
       <c r="B80" s="215" t="s">
         <v>2708</v>
       </c>
       <c r="C80" s="215" t="s">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D80" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E80" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -39014,7 +39011,7 @@
     </row>
     <row r="83" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="19" t="s">
-        <v>3072</v>
+        <v>3071</v>
       </c>
       <c r="B83" s="215" t="s">
         <v>2708</v>
@@ -39026,24 +39023,24 @@
         <v>21</v>
       </c>
       <c r="E83" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
-        <v>3073</v>
+        <v>3072</v>
       </c>
       <c r="B84" s="215" t="s">
         <v>2708</v>
       </c>
       <c r="C84" s="215" t="s">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D84" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E84" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -49486,7 +49483,7 @@
     </row>
     <row r="84" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
-        <v>3074</v>
+        <v>3073</v>
       </c>
       <c r="B84" s="215" t="s">
         <v>2708</v>
@@ -49498,24 +49495,24 @@
         <v>21</v>
       </c>
       <c r="E84" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
-        <v>3075</v>
+        <v>3074</v>
       </c>
       <c r="B85" s="215" t="s">
         <v>2708</v>
       </c>
       <c r="C85" s="215" t="s">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D85" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E85" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -52680,7 +52677,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="206" t="s">
-        <v>3091</v>
+        <v>3090</v>
       </c>
       <c r="B84" s="215" t="s">
         <v>2708</v>
@@ -52692,24 +52689,24 @@
         <v>21</v>
       </c>
       <c r="E84" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="206" t="s">
-        <v>3097</v>
+        <v>3096</v>
       </c>
       <c r="B85" s="215" t="s">
         <v>2708</v>
       </c>
       <c r="C85" s="215" t="s">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D85" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E85" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -60971,7 +60968,7 @@
     </row>
     <row r="83" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="19" t="s">
-        <v>3076</v>
+        <v>3075</v>
       </c>
       <c r="B83" s="215" t="s">
         <v>2708</v>
@@ -60983,24 +60980,24 @@
         <v>21</v>
       </c>
       <c r="E83" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
-        <v>3077</v>
+        <v>3076</v>
       </c>
       <c r="B84" s="215" t="s">
         <v>2708</v>
       </c>
       <c r="C84" s="215" t="s">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D84" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E84" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -62516,7 +62513,7 @@
     </row>
     <row r="85" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
-        <v>3078</v>
+        <v>3077</v>
       </c>
       <c r="B85" s="215" t="s">
         <v>2708</v>
@@ -62528,24 +62525,24 @@
         <v>21</v>
       </c>
       <c r="E85" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="86" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="19" t="s">
-        <v>3079</v>
+        <v>3078</v>
       </c>
       <c r="B86" s="215" t="s">
         <v>2708</v>
       </c>
       <c r="C86" s="215" t="s">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D86" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E86" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -64050,7 +64047,7 @@
     </row>
     <row r="84" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
-        <v>3080</v>
+        <v>3079</v>
       </c>
       <c r="B84" s="215" t="s">
         <v>2708</v>
@@ -64062,24 +64059,24 @@
         <v>21</v>
       </c>
       <c r="E84" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
-        <v>3081</v>
+        <v>3080</v>
       </c>
       <c r="B85" s="215" t="s">
         <v>2708</v>
       </c>
       <c r="C85" s="215" t="s">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D85" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E85" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -65564,7 +65561,7 @@
     </row>
     <row r="83" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="19" t="s">
-        <v>3082</v>
+        <v>3081</v>
       </c>
       <c r="B83" s="215" t="s">
         <v>2708</v>
@@ -65576,24 +65573,24 @@
         <v>21</v>
       </c>
       <c r="E83" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
-        <v>3083</v>
+        <v>3082</v>
       </c>
       <c r="B84" s="215" t="s">
         <v>2708</v>
       </c>
       <c r="C84" s="215" t="s">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D84" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E84" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
   </sheetData>
@@ -67092,7 +67089,7 @@
     </row>
     <row r="84" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
-        <v>3084</v>
+        <v>3083</v>
       </c>
       <c r="B84" s="215" t="s">
         <v>2708</v>
@@ -67104,24 +67101,24 @@
         <v>21</v>
       </c>
       <c r="E84" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
-        <v>3085</v>
+        <v>3084</v>
       </c>
       <c r="B85" s="215" t="s">
         <v>2708</v>
       </c>
       <c r="C85" s="215" t="s">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D85" s="215" t="s">
         <v>21</v>
       </c>
       <c r="E85" s="217" t="s">
-        <v>3067</v>
+        <v>2075</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated OVWSheet with index-Rvar1 YES
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
+++ b/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW-jan14\OVWMigration\docs\OVW Sheets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11010" firstSheet="34" activeTab="41"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11010" firstSheet="35" activeTab="47"/>
   </bookViews>
   <sheets>
     <sheet name="ja_jp" sheetId="48" r:id="rId1"/>
@@ -71,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15499" uniqueCount="3097">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15499" uniqueCount="3098">
   <si>
     <t>products</t>
   </si>
@@ -9362,6 +9357,9 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/ME/solutions/trends/iot/solutions.html</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -10115,7 +10113,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10125,8 +10123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81:E81"/>
+    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10813,7 +10811,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -10830,7 +10828,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -10847,7 +10845,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -10864,7 +10862,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -10881,7 +10879,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -11364,7 +11362,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="215" t="s">
         <v>2849</v>
       </c>
@@ -11582,8 +11580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84:E84"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43:E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12322,7 +12320,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -12339,7 +12337,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -12356,7 +12354,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -12373,7 +12371,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -12390,7 +12388,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -13095,8 +13093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85:E85"/>
+    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13851,7 +13849,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -13868,7 +13866,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -13885,7 +13883,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -13902,7 +13900,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -13919,7 +13917,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -14625,8 +14623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84:E84"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15331,7 +15329,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -15348,7 +15346,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -15365,7 +15363,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -15382,7 +15380,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -15399,7 +15397,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -15895,7 +15893,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="215" t="s">
         <v>2902</v>
       </c>
@@ -15912,7 +15910,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="215" t="s">
         <v>2903</v>
       </c>
@@ -16132,8 +16130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86:E86"/>
+    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16888,7 +16886,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -16905,7 +16903,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -16922,7 +16920,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -16939,7 +16937,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -16956,7 +16954,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -17456,7 +17454,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="215" t="s">
         <v>2908</v>
       </c>
@@ -17681,8 +17679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86:E86"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18437,7 +18435,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -18454,7 +18452,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -18471,7 +18469,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -18488,7 +18486,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -18505,7 +18503,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -19228,8 +19226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71:E71"/>
+    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19984,7 +19982,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -20001,7 +19999,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -20018,7 +20016,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -20035,7 +20033,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -20052,7 +20050,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -20511,8 +20509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69:E69"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21233,7 +21231,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -21250,7 +21248,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -21267,7 +21265,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -21284,7 +21282,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -21301,7 +21299,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -21792,8 +21790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70:E70"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22499,7 +22497,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -22516,7 +22514,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -22533,7 +22531,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -22550,7 +22548,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -22567,7 +22565,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -23052,8 +23050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69:E69"/>
+    <sheetView topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23775,7 +23773,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -23792,7 +23790,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -23809,7 +23807,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -23826,7 +23824,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -23843,7 +23841,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -24303,7 +24301,7 @@
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:E21"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24734,8 +24732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:XFD80"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25423,7 +25421,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -25440,7 +25438,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -25457,7 +25455,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -25474,7 +25472,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -25491,7 +25489,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -25711,7 +25709,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="215" customFormat="1" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="206" t="s">
         <v>2525</v>
       </c>
@@ -25728,7 +25726,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="215" customFormat="1" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="206" t="s">
         <v>2526</v>
       </c>
@@ -25745,7 +25743,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="206" t="s">
         <v>386</v>
       </c>
@@ -25762,7 +25760,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="215" customFormat="1" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="206" t="s">
         <v>391</v>
       </c>
@@ -25779,7 +25777,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="215" customFormat="1" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="181" t="s">
         <v>2645</v>
       </c>
@@ -25793,7 +25791,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="226" t="s">
         <v>2714</v>
       </c>
@@ -25810,7 +25808,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="206" t="s">
         <v>2715</v>
       </c>
@@ -25825,7 +25823,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="205" t="s">
         <v>2716</v>
       </c>
@@ -25842,7 +25840,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="205" t="s">
         <v>2717</v>
       </c>
@@ -25859,7 +25857,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="205" t="s">
         <v>2718</v>
       </c>
@@ -25876,7 +25874,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="216" t="s">
         <v>395</v>
       </c>
@@ -25893,7 +25891,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="216" t="s">
         <v>2719</v>
       </c>
@@ -25906,7 +25904,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="215" t="s">
         <v>2851</v>
       </c>
@@ -25923,7 +25921,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="215" t="s">
         <v>2852</v>
       </c>
@@ -25940,7 +25938,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="215" t="s">
         <v>2853</v>
       </c>
@@ -25957,7 +25955,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="215" t="s">
         <v>2854</v>
       </c>
@@ -25974,7 +25972,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="215" t="s">
         <v>2855</v>
       </c>
@@ -26175,7 +26173,7 @@
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64:E64"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27324,8 +27322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70:E70"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28047,7 +28045,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -28064,7 +28062,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -28081,7 +28079,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -28098,7 +28096,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -28115,7 +28113,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -28584,8 +28582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69:E69"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29307,7 +29305,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -29324,7 +29322,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -29341,7 +29339,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -29358,7 +29356,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -29375,7 +29373,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -29833,8 +29831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68:E68"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30539,7 +30537,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -30556,7 +30554,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -30573,7 +30571,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -30590,7 +30588,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -30607,7 +30605,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -31064,8 +31062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68:E68"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31770,7 +31768,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -31787,7 +31785,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -31804,7 +31802,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -31821,7 +31819,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -31838,7 +31836,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -32296,8 +32294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70:E70"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33019,7 +33017,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -33036,7 +33034,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -33053,7 +33051,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -33070,7 +33068,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -33087,7 +33085,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -33556,8 +33554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66:E66"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38:E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34211,7 +34209,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -34228,7 +34226,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -34245,7 +34243,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -34262,7 +34260,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -34279,7 +34277,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -34745,7 +34743,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:E21"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35132,8 +35130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68:E68"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35855,7 +35853,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -35872,7 +35870,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -35889,7 +35887,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -35906,7 +35904,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -35923,7 +35921,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -36359,8 +36357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70:E70"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37082,7 +37080,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -37099,7 +37097,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -37116,7 +37114,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -37133,7 +37131,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -37150,7 +37148,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -37619,8 +37617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83:E83"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38375,7 +38373,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -38392,7 +38390,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -38409,7 +38407,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -38426,7 +38424,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -38443,7 +38441,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -38731,7 +38729,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="215" customFormat="1" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="181" t="s">
         <v>2646</v>
       </c>
@@ -38745,7 +38743,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="227" t="s">
         <v>2720</v>
       </c>
@@ -38762,7 +38760,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="206" t="s">
         <v>2721</v>
       </c>
@@ -38777,7 +38775,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="206" t="s">
         <v>2722</v>
       </c>
@@ -38794,7 +38792,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="206" t="s">
         <v>2723</v>
       </c>
@@ -38811,7 +38809,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="206" t="s">
         <v>2724</v>
       </c>
@@ -38828,7 +38826,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="205" t="s">
         <v>355</v>
       </c>
@@ -38845,7 +38843,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="182" t="s">
         <v>2725</v>
       </c>
@@ -38858,7 +38856,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="215" t="s">
         <v>2856</v>
       </c>
@@ -38875,7 +38873,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="215" t="s">
         <v>2857</v>
       </c>
@@ -38892,7 +38890,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="215" t="s">
         <v>2858</v>
       </c>
@@ -38909,7 +38907,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="215" t="s">
         <v>2859</v>
       </c>
@@ -39131,8 +39129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70:E70"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39854,7 +39852,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -39871,7 +39869,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -39888,7 +39886,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -39905,7 +39903,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -39922,7 +39920,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -40391,8 +40389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67:E67"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41096,7 +41094,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -41113,7 +41111,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -41130,7 +41128,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -41147,7 +41145,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -41164,7 +41162,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -41608,8 +41606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65:E65"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38:E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42263,7 +42261,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -42280,7 +42278,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -42297,7 +42295,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -42314,7 +42312,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -42331,7 +42329,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -42786,7 +42784,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:E20"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43160,8 +43158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69:E69"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43916,7 +43914,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -43933,7 +43931,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -43950,7 +43948,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -43967,7 +43965,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -43984,7 +43982,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -44413,7 +44411,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:E20"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44788,7 +44786,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:E21"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45179,7 +45177,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:E20"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45553,8 +45551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70:E70"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46309,7 +46307,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -46326,7 +46324,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -46343,7 +46341,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -46360,7 +46358,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -46377,7 +46375,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -46821,8 +46819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69:E69"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47577,7 +47575,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -47594,7 +47592,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -47611,7 +47609,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -47628,7 +47626,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -47645,7 +47643,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -48074,8 +48072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84:XFD85"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48830,7 +48828,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -48847,7 +48845,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -48864,7 +48862,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -48881,7 +48879,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -48898,7 +48896,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -49603,7 +49601,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:E20"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49978,7 +49976,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71:E71"/>
+      <selection activeCell="E44" sqref="E44:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50733,7 +50731,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -50750,7 +50748,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -50767,7 +50765,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -50784,7 +50782,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -50801,7 +50799,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -51268,8 +51266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85:E85"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52024,7 +52022,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -52041,7 +52039,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -52058,7 +52056,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -52075,7 +52073,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -52092,7 +52090,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -52797,8 +52795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71:E71"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53553,7 +53551,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -53570,7 +53568,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -53587,7 +53585,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -53604,7 +53602,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -53621,7 +53619,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -54080,8 +54078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71:E71"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54836,7 +54834,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -54853,7 +54851,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -54870,7 +54868,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -54887,7 +54885,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -54904,7 +54902,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -55363,8 +55361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67:E67"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56068,7 +56066,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -56085,7 +56083,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -56102,7 +56100,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -56119,7 +56117,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -56136,7 +56134,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -56580,8 +56578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57285,7 +57283,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -57302,7 +57300,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -57319,7 +57317,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -57336,7 +57334,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -57353,7 +57351,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -57797,7 +57795,7 @@
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:E28"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58362,8 +58360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59067,7 +59065,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -59084,7 +59082,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -59101,7 +59099,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -59118,7 +59116,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -59135,7 +59133,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -59579,8 +59577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83:XFD84"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60284,7 +60282,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -60301,7 +60299,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -60318,7 +60316,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -60335,7 +60333,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -60352,7 +60350,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -61086,8 +61084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85:XFD86"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61843,7 +61841,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -61860,7 +61858,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -61877,7 +61875,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -61894,7 +61892,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -61911,7 +61909,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -62637,8 +62635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84:XFD85"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63394,7 +63392,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -63411,7 +63409,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -63428,7 +63426,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -63445,7 +63443,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -63462,7 +63460,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -64168,8 +64166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83:XFD84"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64925,7 +64923,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -64942,7 +64940,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -64959,7 +64957,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -64976,7 +64974,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -64993,7 +64991,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -65213,7 +65211,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="199" t="s">
         <v>94</v>
       </c>
@@ -65230,7 +65228,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="215" customFormat="1" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="199" t="s">
         <v>2638</v>
       </c>
@@ -65247,7 +65245,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="215" customFormat="1" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="181" t="s">
         <v>2655</v>
       </c>
@@ -65261,7 +65259,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="215" customFormat="1" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" s="215" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="181" t="s">
         <v>2656</v>
       </c>
@@ -65278,7 +65276,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="226" t="s">
         <v>2750</v>
       </c>
@@ -65295,7 +65293,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="199" t="s">
         <v>2751</v>
       </c>
@@ -65310,7 +65308,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="206" t="s">
         <v>2752</v>
       </c>
@@ -65327,7 +65325,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="206" t="s">
         <v>2753</v>
       </c>
@@ -65344,7 +65342,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="206" t="s">
         <v>2754</v>
       </c>
@@ -65361,7 +65359,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="225" t="s">
         <v>104</v>
       </c>
@@ -65378,7 +65376,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="225" t="s">
         <v>2755</v>
       </c>
@@ -65391,7 +65389,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="215" t="s">
         <v>2880</v>
       </c>
@@ -65408,7 +65406,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="215" t="s">
         <v>2881</v>
       </c>
@@ -65425,7 +65423,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="215" t="s">
         <v>2882</v>
       </c>
@@ -65442,7 +65440,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="215" t="s">
         <v>2883</v>
       </c>
@@ -65459,7 +65457,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="215" t="s">
         <v>2884</v>
       </c>
@@ -65679,8 +65677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -66436,7 +66434,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -66453,7 +66451,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -66470,7 +66468,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -66487,7 +66485,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
@@ -66504,7 +66502,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="217" t="s">
-        <v>2075</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added 3 url's to All URl Sheet.
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
+++ b/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11010" firstSheet="35" activeTab="47"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11010" firstSheet="37" activeTab="47"/>
   </bookViews>
   <sheets>
     <sheet name="ja_jp" sheetId="48" r:id="rId1"/>
@@ -57,16 +57,11 @@
     <sheet name="fr_be" sheetId="4" r:id="rId48"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15499" uniqueCount="3098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16117" uniqueCount="3237">
   <si>
     <t>products</t>
   </si>
@@ -9360,13 +9355,430 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CN/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/cisco/web/UK/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/LA/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/ar/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FR/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FR/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/services/index.html</t>
+  </si>
+  <si>
+    <t>overview-sWebVar10</t>
+  </si>
+  <si>
+    <t>services</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CN/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/cisco/web/UK/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/LA/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/ar/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/services/order-services/index_fr.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ANZ/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IN/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/KR/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/SG/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/NO/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PL/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PT/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ZA/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ES/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/SE/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CH/fr/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CH/de/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TR/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/HK/tc/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/HK/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TW/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/EA/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/nl/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DK/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/EA/services/FR/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IT/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/NL/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TH/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/AT/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/fr/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ID/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/services/index_fr.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ANZ/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IN/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/KR/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/SG/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/NO/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PL/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PT/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RO/products/services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ZA/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ES/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/SE/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CH/fr/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CH/de/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TR/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/UA/products/services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/HK/tc/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/HK/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TW/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/EA/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IL/products/services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/GR/products/services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/nl/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FI/products/services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BG/products/services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CZ/products/services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DK/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/EA/services/FR/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.cisco.com/web/HU/termekek_es_megoldasok/services.html </t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IT/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/NL/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TH/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/AT/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/fr/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ID/services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/cisco/web/UK/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/LA/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/ar/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FR/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/midsize/index_fr.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ANZ/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IN/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/KR/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/SG/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/NO/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PL/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PT/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RO/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ZA/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ES/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/SE/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CH/fr/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CH/de/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TR/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/UA/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/UA/uk/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/HK/tc/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/HK/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TW/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/EA/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IL/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/GR/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/nl/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FI/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BG/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CZ/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DK/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/EA/midsize/FR/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/HU/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IT/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/NL/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TH/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/AT/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/fr/midsize/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ID/midsize/index.html</t>
+  </si>
+  <si>
+    <t>order-services</t>
+  </si>
+  <si>
+    <t>order-services-webvar11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">overview-WebVar3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">midsize </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9411,6 +9823,19 @@
     </font>
     <font>
       <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -9551,7 +9976,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="229">
+  <cellXfs count="252">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -9811,6 +10236,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="31">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9850,9 +10302,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -10113,7 +10562,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10121,10 +10570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11493,6 +11942,54 @@
         <v>21</v>
       </c>
       <c r="E81" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="236" t="s">
+        <v>3105</v>
+      </c>
+      <c r="B82" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C82" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D82" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E82" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="241" t="s">
+        <v>3108</v>
+      </c>
+      <c r="C83" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D83" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E83" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="250" t="s">
+        <v>3187</v>
+      </c>
+      <c r="B84" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C84" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D84" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -11570,18 +12067,21 @@
     <hyperlink ref="A77" r:id="rId70"/>
     <hyperlink ref="A80" r:id="rId71"/>
     <hyperlink ref="A81" r:id="rId72"/>
+    <hyperlink ref="A82" r:id="rId73"/>
+    <hyperlink ref="A83" r:id="rId74"/>
+    <hyperlink ref="A84" r:id="rId75"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId73"/>
+  <pageSetup orientation="portrait" r:id="rId76"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43:E47"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85:E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13002,6 +13502,55 @@
         <v>21</v>
       </c>
       <c r="E84" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="251" t="s">
+        <v>3119</v>
+      </c>
+      <c r="B85" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C85" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D85" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E85" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="251" t="s">
+        <v>3149</v>
+      </c>
+      <c r="B86" s="248"/>
+      <c r="C86" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D86" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E86" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="251" t="s">
+        <v>3194</v>
+      </c>
+      <c r="B87" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C87" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D87" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E87" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -13084,6 +13633,9 @@
     <hyperlink ref="A81" r:id="rId75"/>
     <hyperlink ref="A83" r:id="rId76"/>
     <hyperlink ref="A84" r:id="rId77"/>
+    <hyperlink ref="A85" r:id="rId78"/>
+    <hyperlink ref="A86" r:id="rId79"/>
+    <hyperlink ref="A87" r:id="rId80"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13091,10 +13643,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E48"/>
+    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86:E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14531,6 +15083,55 @@
         <v>21</v>
       </c>
       <c r="E85" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="251" t="s">
+        <v>3120</v>
+      </c>
+      <c r="B86" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C86" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D86" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E86" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="251" t="s">
+        <v>3150</v>
+      </c>
+      <c r="B87" s="248"/>
+      <c r="C87" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D87" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E87" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="251" t="s">
+        <v>3195</v>
+      </c>
+      <c r="B88" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C88" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D88" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E88" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -14614,6 +15215,9 @@
     <hyperlink ref="A82" r:id="rId76"/>
     <hyperlink ref="A84" r:id="rId77"/>
     <hyperlink ref="A85" r:id="rId78"/>
+    <hyperlink ref="A86" r:id="rId79"/>
+    <hyperlink ref="A87" r:id="rId80"/>
+    <hyperlink ref="A88" r:id="rId81"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14621,10 +15225,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41:E45"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85:E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16041,6 +16645,55 @@
         <v>21</v>
       </c>
       <c r="E84" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="251" t="s">
+        <v>3121</v>
+      </c>
+      <c r="B85" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C85" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D85" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E85" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="251" t="s">
+        <v>3151</v>
+      </c>
+      <c r="B86" s="248"/>
+      <c r="C86" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D86" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E86" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="251" t="s">
+        <v>3196</v>
+      </c>
+      <c r="B87" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C87" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D87" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E87" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -16121,6 +16774,9 @@
     <hyperlink ref="A81" r:id="rId73"/>
     <hyperlink ref="A83" r:id="rId74"/>
     <hyperlink ref="A84" r:id="rId75"/>
+    <hyperlink ref="A85" r:id="rId76"/>
+    <hyperlink ref="A86" r:id="rId77"/>
+    <hyperlink ref="A87" r:id="rId78"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16128,10 +16784,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E48"/>
+    <sheetView topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87:E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17585,6 +18241,55 @@
         <v>21</v>
       </c>
       <c r="E86" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="251" t="s">
+        <v>3122</v>
+      </c>
+      <c r="B87" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C87" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D87" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E87" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="251" t="s">
+        <v>3152</v>
+      </c>
+      <c r="B88" s="248"/>
+      <c r="C88" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D88" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E88" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="251" t="s">
+        <v>3197</v>
+      </c>
+      <c r="B89" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C89" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D89" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E89" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -17669,18 +18374,21 @@
     <hyperlink ref="A83" r:id="rId77"/>
     <hyperlink ref="A85" r:id="rId78"/>
     <hyperlink ref="A86" r:id="rId79"/>
+    <hyperlink ref="A87" r:id="rId80"/>
+    <hyperlink ref="A88" r:id="rId81"/>
+    <hyperlink ref="A89" r:id="rId82"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId80"/>
+  <pageSetup orientation="portrait" r:id="rId83"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E48"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87:E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19134,6 +19842,55 @@
         <v>21</v>
       </c>
       <c r="E86" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="251" t="s">
+        <v>3123</v>
+      </c>
+      <c r="B87" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C87" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D87" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E87" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="251" t="s">
+        <v>3153</v>
+      </c>
+      <c r="B88" s="248"/>
+      <c r="C88" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D88" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E88" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="251" t="s">
+        <v>3198</v>
+      </c>
+      <c r="B89" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C89" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D89" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E89" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -19217,6 +19974,9 @@
     <hyperlink ref="A83" r:id="rId76"/>
     <hyperlink ref="A85" r:id="rId77"/>
     <hyperlink ref="A86" r:id="rId78"/>
+    <hyperlink ref="A87" r:id="rId79"/>
+    <hyperlink ref="A88" r:id="rId80"/>
+    <hyperlink ref="A89" r:id="rId81"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19224,10 +19984,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E48"/>
+    <sheetView topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20426,6 +21186,55 @@
         <v>21</v>
       </c>
       <c r="E71" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="250" t="s">
+        <v>3124</v>
+      </c>
+      <c r="B72" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C72" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D72" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E72" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="250" t="s">
+        <v>3154</v>
+      </c>
+      <c r="B73" s="248"/>
+      <c r="C73" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D73" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E73" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="250" t="s">
+        <v>3199</v>
+      </c>
+      <c r="B74" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C74" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D74" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -20500,6 +21309,9 @@
     <hyperlink ref="A67" r:id="rId67"/>
     <hyperlink ref="A68" r:id="rId68"/>
     <hyperlink ref="A71" r:id="rId69"/>
+    <hyperlink ref="A72" r:id="rId70"/>
+    <hyperlink ref="A73" r:id="rId71"/>
+    <hyperlink ref="A74" r:id="rId72"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20509,8 +21321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42:E46"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70:E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21683,22 +22495,53 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="206"/>
-      <c r="B70" s="215"/>
-      <c r="C70" s="215"/>
-      <c r="D70" s="215"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="206"/>
-      <c r="B71" s="215"/>
-      <c r="C71" s="215"/>
-      <c r="D71" s="215"/>
+      <c r="A70" s="251" t="s">
+        <v>3125</v>
+      </c>
+      <c r="B70" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C70" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D70" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E70" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="251" t="s">
+        <v>3155</v>
+      </c>
+      <c r="B71" s="248"/>
+      <c r="C71" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D71" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E71" s="249" t="s">
+        <v>2075</v>
+      </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="206"/>
-      <c r="B72" s="215"/>
-      <c r="C72" s="215"/>
-      <c r="D72" s="215"/>
+      <c r="A72" s="251" t="s">
+        <v>3200</v>
+      </c>
+      <c r="B72" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C72" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D72" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" s="249" t="s">
+        <v>2075</v>
+      </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="206"/>
@@ -21781,6 +22624,9 @@
     <hyperlink ref="A66" r:id="rId65"/>
     <hyperlink ref="A67" r:id="rId66"/>
     <hyperlink ref="A69" r:id="rId67"/>
+    <hyperlink ref="A70" r:id="rId68"/>
+    <hyperlink ref="A71" r:id="rId69"/>
+    <hyperlink ref="A72" r:id="rId70"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21788,10 +22634,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41:E45"/>
+      <selection activeCell="B71" sqref="B71:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22969,6 +23815,55 @@
         <v>21</v>
       </c>
       <c r="E70" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="251" t="s">
+        <v>3126</v>
+      </c>
+      <c r="B71" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C71" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D71" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E71" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="251" t="s">
+        <v>3156</v>
+      </c>
+      <c r="B72" s="248"/>
+      <c r="C72" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D72" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E72" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="251" t="s">
+        <v>3201</v>
+      </c>
+      <c r="B73" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C73" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D73" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -23041,6 +23936,9 @@
     <hyperlink ref="A66" r:id="rId65"/>
     <hyperlink ref="A67" r:id="rId66"/>
     <hyperlink ref="A70" r:id="rId67"/>
+    <hyperlink ref="A71" r:id="rId68"/>
+    <hyperlink ref="A72" r:id="rId69"/>
+    <hyperlink ref="A73" r:id="rId70"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -23048,10 +23946,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42:E46"/>
+      <selection activeCell="B70" sqref="B70:E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24217,6 +25115,55 @@
         <v>21</v>
       </c>
       <c r="E69" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="251" t="s">
+        <v>3127</v>
+      </c>
+      <c r="B70" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C70" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D70" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E70" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="251" t="s">
+        <v>3157</v>
+      </c>
+      <c r="B71" s="248"/>
+      <c r="C71" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D71" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E71" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="250" t="s">
+        <v>3202</v>
+      </c>
+      <c r="B72" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C72" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D72" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -24291,6 +25238,9 @@
     <hyperlink ref="A66" r:id="rId67"/>
     <hyperlink ref="A67" r:id="rId68"/>
     <hyperlink ref="A69" r:id="rId69"/>
+    <hyperlink ref="A70" r:id="rId70"/>
+    <hyperlink ref="A71" r:id="rId71"/>
+    <hyperlink ref="A72" r:id="rId72"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24301,7 +25251,7 @@
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B22" sqref="B22:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24657,6 +25607,44 @@
       <c r="E21" s="217" t="s">
         <v>2075</v>
       </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="251" t="s">
+        <v>3158</v>
+      </c>
+      <c r="B22" s="248"/>
+      <c r="C22" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D22" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E22" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="251" t="s">
+        <v>3203</v>
+      </c>
+      <c r="B23" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C23" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D23" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="248"/>
+      <c r="C24" s="248"/>
+      <c r="D24" s="248"/>
+      <c r="E24" s="249"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="215" t="s">
@@ -24723,6 +25711,8 @@
     <hyperlink ref="A18" r:id="rId19"/>
     <hyperlink ref="A19" r:id="rId20"/>
     <hyperlink ref="A21" r:id="rId21"/>
+    <hyperlink ref="A22" r:id="rId22"/>
+    <hyperlink ref="A23" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24730,10 +25720,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40:E44"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83:E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26088,6 +27078,44 @@
       <c r="E80" s="217" t="s">
         <v>2075</v>
       </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="230" t="s">
+        <v>3099</v>
+      </c>
+      <c r="B81" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C81" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D81" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E81" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="243" t="s">
+        <v>3112</v>
+      </c>
+      <c r="B82" s="248"/>
+      <c r="C82" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D82" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E82" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B83" s="248"/>
+      <c r="C83" s="248"/>
+      <c r="D83" s="248"/>
+      <c r="E83" s="249"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -26163,6 +27191,8 @@
     <hyperlink ref="A77" r:id="rId70"/>
     <hyperlink ref="A79" r:id="rId71"/>
     <hyperlink ref="A80" r:id="rId72"/>
+    <hyperlink ref="A81" r:id="rId73"/>
+    <hyperlink ref="A82" r:id="rId74"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -26170,10 +27200,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="B65" sqref="B65:E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27253,6 +28283,55 @@
         <v>21</v>
       </c>
       <c r="E64" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="251" t="s">
+        <v>3128</v>
+      </c>
+      <c r="B65" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C65" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D65" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E65" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="251" t="s">
+        <v>3159</v>
+      </c>
+      <c r="B66" s="248"/>
+      <c r="C66" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D66" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E66" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="251" t="s">
+        <v>3204</v>
+      </c>
+      <c r="B67" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C67" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D67" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -27313,6 +28392,9 @@
     <hyperlink ref="A60" r:id="rId53"/>
     <hyperlink ref="A61" r:id="rId54"/>
     <hyperlink ref="A64" r:id="rId55"/>
+    <hyperlink ref="A65" r:id="rId56"/>
+    <hyperlink ref="A66" r:id="rId57"/>
+    <hyperlink ref="A67" r:id="rId58"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -27320,10 +28402,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42:E46"/>
+      <selection activeCell="B71" sqref="B71:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28500,6 +29582,55 @@
         <v>21</v>
       </c>
       <c r="E70" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="251" t="s">
+        <v>3129</v>
+      </c>
+      <c r="B71" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C71" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D71" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E71" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="251" t="s">
+        <v>3160</v>
+      </c>
+      <c r="B72" s="248"/>
+      <c r="C72" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D72" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E72" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="251" t="s">
+        <v>3205</v>
+      </c>
+      <c r="B73" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C73" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D73" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -28573,6 +29704,9 @@
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
     <hyperlink ref="A70" r:id="rId68"/>
+    <hyperlink ref="A71" r:id="rId69"/>
+    <hyperlink ref="A72" r:id="rId70"/>
+    <hyperlink ref="A73" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28580,10 +29714,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42:E46"/>
+      <selection activeCell="B70" sqref="B70:E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29749,6 +30883,55 @@
         <v>21</v>
       </c>
       <c r="E69" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="251" t="s">
+        <v>3130</v>
+      </c>
+      <c r="B70" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C70" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D70" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E70" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="251" t="s">
+        <v>3161</v>
+      </c>
+      <c r="B71" s="248"/>
+      <c r="C71" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D71" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E71" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="251" t="s">
+        <v>3206</v>
+      </c>
+      <c r="B72" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C72" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D72" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -29822,6 +31005,9 @@
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
     <hyperlink ref="A69" r:id="rId68"/>
+    <hyperlink ref="A70" r:id="rId69"/>
+    <hyperlink ref="A71" r:id="rId70"/>
+    <hyperlink ref="A72" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29829,10 +31015,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41:E45"/>
+      <selection activeCell="B69" sqref="B69:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30981,6 +32167,55 @@
         <v>21</v>
       </c>
       <c r="E68" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="250" t="s">
+        <v>3131</v>
+      </c>
+      <c r="B69" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C69" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D69" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E69" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="250" t="s">
+        <v>3162</v>
+      </c>
+      <c r="B70" s="248"/>
+      <c r="C70" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D70" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E70" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="250" t="s">
+        <v>3207</v>
+      </c>
+      <c r="B71" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C71" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D71" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -31053,6 +32288,9 @@
     <hyperlink ref="A65" r:id="rId65"/>
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A68" r:id="rId67"/>
+    <hyperlink ref="A69" r:id="rId68"/>
+    <hyperlink ref="A70" r:id="rId69"/>
+    <hyperlink ref="A71" r:id="rId70"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -31060,10 +32298,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41:E45"/>
+      <selection activeCell="B69" sqref="B69:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32212,6 +33450,55 @@
         <v>21</v>
       </c>
       <c r="E68" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="250" t="s">
+        <v>3132</v>
+      </c>
+      <c r="B69" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C69" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D69" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E69" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="250" t="s">
+        <v>3163</v>
+      </c>
+      <c r="B70" s="248"/>
+      <c r="C70" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D70" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E70" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="250" t="s">
+        <v>3208</v>
+      </c>
+      <c r="B71" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C71" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D71" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -32285,6 +33572,9 @@
     <hyperlink ref="A65" r:id="rId66"/>
     <hyperlink ref="A66" r:id="rId67"/>
     <hyperlink ref="A68" r:id="rId68"/>
+    <hyperlink ref="A69" r:id="rId69"/>
+    <hyperlink ref="A70" r:id="rId70"/>
+    <hyperlink ref="A71" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -32292,10 +33582,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42:E46"/>
+      <selection activeCell="B71" sqref="B71:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33472,6 +34762,55 @@
         <v>21</v>
       </c>
       <c r="E70" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="251" t="s">
+        <v>3133</v>
+      </c>
+      <c r="B71" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C71" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D71" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E71" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="251" t="s">
+        <v>3164</v>
+      </c>
+      <c r="B72" s="248"/>
+      <c r="C72" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D72" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E72" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="251" t="s">
+        <v>3209</v>
+      </c>
+      <c r="B73" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C73" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D73" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -33545,6 +34884,9 @@
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
     <hyperlink ref="A70" r:id="rId68"/>
+    <hyperlink ref="A71" r:id="rId69"/>
+    <hyperlink ref="A72" r:id="rId70"/>
+    <hyperlink ref="A73" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33552,10 +34894,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:E42"/>
+      <selection activeCell="B67" sqref="B67:E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34664,6 +36006,38 @@
         <v>21</v>
       </c>
       <c r="E66" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="251" t="s">
+        <v>3165</v>
+      </c>
+      <c r="B67" s="248"/>
+      <c r="C67" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D67" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E67" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="251" t="s">
+        <v>3210</v>
+      </c>
+      <c r="B68" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C68" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D68" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E68" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -34733,6 +36107,8 @@
     <hyperlink ref="A62" r:id="rId62"/>
     <hyperlink ref="A63" r:id="rId63"/>
     <hyperlink ref="A66" r:id="rId64"/>
+    <hyperlink ref="A67" r:id="rId65"/>
+    <hyperlink ref="A68" r:id="rId66"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34740,10 +36116,10 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B23" sqref="B23:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35098,6 +36474,29 @@
       <c r="E21" s="217" t="s">
         <v>2075</v>
       </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="250" t="s">
+        <v>3211</v>
+      </c>
+      <c r="B22" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C22" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D22" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="248"/>
+      <c r="C23" s="238"/>
+      <c r="D23" s="239"/>
+      <c r="E23" s="249"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -35121,6 +36520,7 @@
     <hyperlink ref="A17" r:id="rId18"/>
     <hyperlink ref="A18" r:id="rId19"/>
     <hyperlink ref="A21" r:id="rId20"/>
+    <hyperlink ref="A22" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -35128,10 +36528,10 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42:E46"/>
+      <selection activeCell="B69" sqref="B69:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36277,6 +37677,55 @@
         <v>21</v>
       </c>
       <c r="E68" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="251" t="s">
+        <v>3134</v>
+      </c>
+      <c r="B69" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C69" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D69" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E69" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="251" t="s">
+        <v>3166</v>
+      </c>
+      <c r="B70" s="248"/>
+      <c r="C70" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D70" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E70" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="251" t="s">
+        <v>3212</v>
+      </c>
+      <c r="B71" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C71" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D71" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -36348,6 +37797,8 @@
     <hyperlink ref="A64" r:id="rId64"/>
     <hyperlink ref="A65" r:id="rId65"/>
     <hyperlink ref="A68" r:id="rId66"/>
+    <hyperlink ref="A69" r:id="rId67"/>
+    <hyperlink ref="A71" r:id="rId68"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -36355,10 +37806,10 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42:E46"/>
+      <selection activeCell="B71" sqref="B71:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37535,6 +38986,55 @@
         <v>21</v>
       </c>
       <c r="E70" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="251" t="s">
+        <v>3135</v>
+      </c>
+      <c r="B71" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C71" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D71" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E71" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="251" t="s">
+        <v>3167</v>
+      </c>
+      <c r="B72" s="248"/>
+      <c r="C72" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D72" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E72" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="251" t="s">
+        <v>3213</v>
+      </c>
+      <c r="B73" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C73" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D73" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -37608,6 +39108,9 @@
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
     <hyperlink ref="A70" r:id="rId68"/>
+    <hyperlink ref="A71" r:id="rId69"/>
+    <hyperlink ref="A72" r:id="rId70"/>
+    <hyperlink ref="A73" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -37615,10 +39118,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E48"/>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85:E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39038,6 +40541,55 @@
         <v>21</v>
       </c>
       <c r="E84" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="231" t="s">
+        <v>3100</v>
+      </c>
+      <c r="B85" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C85" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D85" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E85" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="244" t="s">
+        <v>3113</v>
+      </c>
+      <c r="B86" s="248"/>
+      <c r="C86" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D86" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E86" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="251" t="s">
+        <v>3188</v>
+      </c>
+      <c r="B87" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C87" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D87" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E87" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -39120,6 +40672,9 @@
     <hyperlink ref="A81" r:id="rId75"/>
     <hyperlink ref="A83" r:id="rId76"/>
     <hyperlink ref="A84" r:id="rId77"/>
+    <hyperlink ref="A85" r:id="rId78"/>
+    <hyperlink ref="A86" r:id="rId79"/>
+    <hyperlink ref="A87" r:id="rId80"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -39127,10 +40682,10 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42:E46"/>
+      <selection activeCell="B71" sqref="B71:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40307,6 +41862,55 @@
         <v>21</v>
       </c>
       <c r="E70" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="251" t="s">
+        <v>3136</v>
+      </c>
+      <c r="B71" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C71" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D71" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E71" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="251" t="s">
+        <v>3168</v>
+      </c>
+      <c r="B72" s="248"/>
+      <c r="C72" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D72" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E72" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="251" t="s">
+        <v>3214</v>
+      </c>
+      <c r="B73" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C73" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D73" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -40380,6 +41984,9 @@
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
     <hyperlink ref="A70" r:id="rId68"/>
+    <hyperlink ref="A71" r:id="rId69"/>
+    <hyperlink ref="A72" r:id="rId70"/>
+    <hyperlink ref="A73" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -40387,10 +41994,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41:E45"/>
+      <selection activeCell="B68" sqref="B68:E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41525,6 +43132,55 @@
         <v>21</v>
       </c>
       <c r="E67" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="251" t="s">
+        <v>3137</v>
+      </c>
+      <c r="B68" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C68" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D68" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E68" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="251" t="s">
+        <v>3169</v>
+      </c>
+      <c r="B69" s="248"/>
+      <c r="C69" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D69" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E69" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="251" t="s">
+        <v>3215</v>
+      </c>
+      <c r="B70" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C70" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D70" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -41597,6 +43253,9 @@
     <hyperlink ref="A64" r:id="rId65"/>
     <hyperlink ref="A65" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
+    <hyperlink ref="A68" r:id="rId68"/>
+    <hyperlink ref="A69" r:id="rId69"/>
+    <hyperlink ref="A70" r:id="rId70"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -41604,10 +43263,10 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:E42"/>
+      <selection activeCell="B66" sqref="B66:E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42707,6 +44366,44 @@
       <c r="E65" s="217" t="s">
         <v>2075</v>
       </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="251" t="s">
+        <v>3170</v>
+      </c>
+      <c r="B66" s="248"/>
+      <c r="C66" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D66" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E66" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="251" t="s">
+        <v>3216</v>
+      </c>
+      <c r="B67" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C67" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D67" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="248"/>
+      <c r="C68" s="248"/>
+      <c r="D68" s="248"/>
+      <c r="E68" s="249"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -42774,6 +44471,8 @@
     <hyperlink ref="A62" r:id="rId62"/>
     <hyperlink ref="A63" r:id="rId63"/>
     <hyperlink ref="A65" r:id="rId64"/>
+    <hyperlink ref="A66" r:id="rId65"/>
+    <hyperlink ref="A67" r:id="rId66"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -42781,10 +44480,10 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B21" sqref="B21:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43126,6 +44825,44 @@
       <c r="E20" s="217" t="s">
         <v>2075</v>
       </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="251" t="s">
+        <v>3171</v>
+      </c>
+      <c r="B21" s="248"/>
+      <c r="C21" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D21" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E21" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="251" t="s">
+        <v>3217</v>
+      </c>
+      <c r="B22" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C22" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D22" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="248"/>
+      <c r="C23" s="248"/>
+      <c r="D23" s="248"/>
+      <c r="E23" s="249"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -43149,6 +44886,8 @@
     <hyperlink ref="A17" r:id="rId18"/>
     <hyperlink ref="A18" r:id="rId19"/>
     <hyperlink ref="A20" r:id="rId20"/>
+    <hyperlink ref="A21" r:id="rId21"/>
+    <hyperlink ref="A22" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -43156,10 +44895,10 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E48"/>
+      <selection activeCell="B70" sqref="B70:E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44328,6 +46067,55 @@
         <v>21</v>
       </c>
       <c r="E69" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="250" t="s">
+        <v>3138</v>
+      </c>
+      <c r="B70" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C70" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D70" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E70" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="250" t="s">
+        <v>3172</v>
+      </c>
+      <c r="B71" s="248"/>
+      <c r="C71" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D71" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E71" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="250" t="s">
+        <v>3218</v>
+      </c>
+      <c r="B72" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C72" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D72" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -44401,6 +46189,9 @@
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
     <hyperlink ref="A69" r:id="rId68"/>
+    <hyperlink ref="A70" r:id="rId69"/>
+    <hyperlink ref="A71" r:id="rId70"/>
+    <hyperlink ref="A72" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -44408,10 +46199,10 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B21" sqref="B21:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44753,6 +46544,44 @@
       <c r="E20" s="217" t="s">
         <v>2075</v>
       </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="251" t="s">
+        <v>3173</v>
+      </c>
+      <c r="B21" s="248"/>
+      <c r="C21" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D21" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E21" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="251" t="s">
+        <v>3219</v>
+      </c>
+      <c r="B22" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C22" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D22" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="248"/>
+      <c r="C23" s="248"/>
+      <c r="D23" s="248"/>
+      <c r="E23" s="249"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -44776,6 +46605,8 @@
     <hyperlink ref="A17" r:id="rId18"/>
     <hyperlink ref="A18" r:id="rId19"/>
     <hyperlink ref="A20" r:id="rId20"/>
+    <hyperlink ref="A21" r:id="rId21"/>
+    <hyperlink ref="A22" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -44783,10 +46614,10 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B22" sqref="B22:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45143,6 +46974,44 @@
       <c r="E21" s="217" t="s">
         <v>2075</v>
       </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="251" t="s">
+        <v>3174</v>
+      </c>
+      <c r="B22" s="248"/>
+      <c r="C22" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D22" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E22" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="251" t="s">
+        <v>3220</v>
+      </c>
+      <c r="B23" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C23" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D23" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="248"/>
+      <c r="C24" s="248"/>
+      <c r="D24" s="248"/>
+      <c r="E24" s="249"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -45167,6 +47036,8 @@
     <hyperlink ref="A18" r:id="rId19"/>
     <hyperlink ref="A19" r:id="rId20"/>
     <hyperlink ref="A21" r:id="rId21"/>
+    <hyperlink ref="A22" r:id="rId22"/>
+    <hyperlink ref="A23" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -45174,10 +47045,10 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B21" sqref="B21:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45517,6 +47388,38 @@
         <v>21</v>
       </c>
       <c r="E20" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="251" t="s">
+        <v>3175</v>
+      </c>
+      <c r="B21" s="248"/>
+      <c r="C21" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D21" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E21" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="251" t="s">
+        <v>3221</v>
+      </c>
+      <c r="B22" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C22" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D22" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -45542,6 +47445,8 @@
     <hyperlink ref="A17" r:id="rId18"/>
     <hyperlink ref="A18" r:id="rId19"/>
     <hyperlink ref="A20" r:id="rId20"/>
+    <hyperlink ref="A21" r:id="rId21"/>
+    <hyperlink ref="A22" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -45549,10 +47454,10 @@
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E48"/>
+      <selection activeCell="B71" sqref="B71:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46738,6 +48643,55 @@
         <v>21</v>
       </c>
       <c r="E70" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="251" t="s">
+        <v>3139</v>
+      </c>
+      <c r="B71" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C71" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D71" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E71" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="251" t="s">
+        <v>3176</v>
+      </c>
+      <c r="B72" s="248"/>
+      <c r="C72" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D72" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E72" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="251" t="s">
+        <v>3222</v>
+      </c>
+      <c r="B73" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C73" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D73" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -46810,6 +48764,9 @@
     <hyperlink ref="A67" r:id="rId65"/>
     <hyperlink ref="A68" r:id="rId66"/>
     <hyperlink ref="A70" r:id="rId67"/>
+    <hyperlink ref="A71" r:id="rId68"/>
+    <hyperlink ref="A72" r:id="rId69"/>
+    <hyperlink ref="A73" r:id="rId70"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -46817,10 +48774,10 @@
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E48"/>
+      <selection activeCell="B70" sqref="B70:E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47989,6 +49946,55 @@
         <v>21</v>
       </c>
       <c r="E69" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="250" t="s">
+        <v>3140</v>
+      </c>
+      <c r="B70" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C70" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D70" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E70" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="250" t="s">
+        <v>3177</v>
+      </c>
+      <c r="B71" s="248"/>
+      <c r="C71" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D71" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E71" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="251" t="s">
+        <v>3223</v>
+      </c>
+      <c r="B72" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C72" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D72" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -48063,6 +50069,9 @@
     <hyperlink ref="A66" r:id="rId67"/>
     <hyperlink ref="A67" r:id="rId68"/>
     <hyperlink ref="A69" r:id="rId69"/>
+    <hyperlink ref="A70" r:id="rId70"/>
+    <hyperlink ref="A71" r:id="rId71"/>
+    <hyperlink ref="A72" r:id="rId72"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -48070,10 +50079,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E48"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86:E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49510,6 +51519,55 @@
         <v>21</v>
       </c>
       <c r="E85" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="232" t="s">
+        <v>3101</v>
+      </c>
+      <c r="B86" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C86" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D86" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E86" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="245" t="s">
+        <v>3114</v>
+      </c>
+      <c r="B87" s="248"/>
+      <c r="C87" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D87" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E87" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="251" t="s">
+        <v>3189</v>
+      </c>
+      <c r="B88" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C88" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D88" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E88" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -49591,6 +51649,9 @@
     <hyperlink ref="A82" r:id="rId74"/>
     <hyperlink ref="A84" r:id="rId75"/>
     <hyperlink ref="A85" r:id="rId76"/>
+    <hyperlink ref="A86" r:id="rId77"/>
+    <hyperlink ref="A87" r:id="rId78"/>
+    <hyperlink ref="A88" r:id="rId79"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -49598,15 +51659,15 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.42578125" customWidth="1"/>
+    <col min="1" max="1" width="70.42578125" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
   </cols>
@@ -49941,6 +52002,38 @@
         <v>21</v>
       </c>
       <c r="E20" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="251" t="s">
+        <v>3178</v>
+      </c>
+      <c r="B21" s="248"/>
+      <c r="C21" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D21" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E21" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="251" t="s">
+        <v>3224</v>
+      </c>
+      <c r="B22" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C22" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D22" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -49966,6 +52059,8 @@
     <hyperlink ref="A17" r:id="rId18"/>
     <hyperlink ref="A18" r:id="rId19"/>
     <hyperlink ref="A20" r:id="rId20"/>
+    <hyperlink ref="A21" r:id="rId21"/>
+    <hyperlink ref="A22" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -49973,10 +52068,10 @@
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E48"/>
+      <selection activeCell="B72" sqref="B72:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51181,6 +53276,55 @@
         <v>21</v>
       </c>
       <c r="E71" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="251" t="s">
+        <v>3141</v>
+      </c>
+      <c r="B72" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C72" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D72" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E72" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="251" t="s">
+        <v>3179</v>
+      </c>
+      <c r="B73" s="248"/>
+      <c r="C73" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D73" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E73" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="251" t="s">
+        <v>3225</v>
+      </c>
+      <c r="B74" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C74" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D74" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -51257,6 +53401,9 @@
     <hyperlink ref="A69" r:id="rId69"/>
     <hyperlink ref="A70" r:id="rId70"/>
     <hyperlink ref="A71" r:id="rId71"/>
+    <hyperlink ref="A72" r:id="rId72"/>
+    <hyperlink ref="A73" r:id="rId73"/>
+    <hyperlink ref="A74" r:id="rId74"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -51264,10 +53411,10 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E48"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86:E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52704,6 +54851,55 @@
         <v>21</v>
       </c>
       <c r="E85" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="251" t="s">
+        <v>3142</v>
+      </c>
+      <c r="B86" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C86" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D86" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E86" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="251" t="s">
+        <v>3180</v>
+      </c>
+      <c r="B87" s="248"/>
+      <c r="C87" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D87" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E87" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="251" t="s">
+        <v>3226</v>
+      </c>
+      <c r="B88" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C88" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D88" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E88" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -52786,6 +54982,9 @@
     <hyperlink ref="A82" r:id="rId75"/>
     <hyperlink ref="A84" r:id="rId76"/>
     <hyperlink ref="A85" r:id="rId77"/>
+    <hyperlink ref="A86" r:id="rId78"/>
+    <hyperlink ref="A87" r:id="rId79"/>
+    <hyperlink ref="A88" r:id="rId80"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -52793,10 +54992,10 @@
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E48"/>
+      <selection activeCell="B72" sqref="B72:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53995,6 +56194,55 @@
         <v>21</v>
       </c>
       <c r="E71" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="250" t="s">
+        <v>3143</v>
+      </c>
+      <c r="B72" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C72" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D72" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E72" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="250" t="s">
+        <v>3181</v>
+      </c>
+      <c r="B73" s="248"/>
+      <c r="C73" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D73" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E73" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="251" t="s">
+        <v>3227</v>
+      </c>
+      <c r="B74" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C74" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D74" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -54069,6 +56317,9 @@
     <hyperlink ref="A67" r:id="rId67"/>
     <hyperlink ref="A68" r:id="rId68"/>
     <hyperlink ref="A71" r:id="rId69"/>
+    <hyperlink ref="A72" r:id="rId70"/>
+    <hyperlink ref="A73" r:id="rId71"/>
+    <hyperlink ref="A74" r:id="rId72"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -54076,10 +56327,10 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E48"/>
+      <selection activeCell="B72" sqref="B72:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55278,6 +57529,55 @@
         <v>21</v>
       </c>
       <c r="E71" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="251" t="s">
+        <v>3144</v>
+      </c>
+      <c r="B72" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C72" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D72" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E72" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="251" t="s">
+        <v>3182</v>
+      </c>
+      <c r="B73" s="248"/>
+      <c r="C73" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D73" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E73" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="251" t="s">
+        <v>3228</v>
+      </c>
+      <c r="B74" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C74" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D74" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -55352,6 +57652,9 @@
     <hyperlink ref="A67" r:id="rId67"/>
     <hyperlink ref="A68" r:id="rId68"/>
     <hyperlink ref="A71" r:id="rId69"/>
+    <hyperlink ref="A72" r:id="rId70"/>
+    <hyperlink ref="A73" r:id="rId71"/>
+    <hyperlink ref="A74" r:id="rId72"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -55359,10 +57662,10 @@
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41:E45"/>
+      <selection activeCell="B68" sqref="B68:E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56497,6 +58800,55 @@
         <v>21</v>
       </c>
       <c r="E67" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="251" t="s">
+        <v>3145</v>
+      </c>
+      <c r="B68" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C68" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D68" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E68" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="251" t="s">
+        <v>3183</v>
+      </c>
+      <c r="B69" s="248"/>
+      <c r="C69" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D69" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E69" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="251" t="s">
+        <v>3229</v>
+      </c>
+      <c r="B70" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C70" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D70" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -56569,6 +58921,9 @@
     <hyperlink ref="A65" r:id="rId65"/>
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
+    <hyperlink ref="A68" r:id="rId68"/>
+    <hyperlink ref="A69" r:id="rId69"/>
+    <hyperlink ref="A70" r:id="rId70"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -56576,10 +58931,10 @@
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41:E45"/>
+      <selection activeCell="B68" sqref="B68:E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57714,6 +60069,55 @@
         <v>21</v>
       </c>
       <c r="E67" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="251" t="s">
+        <v>3146</v>
+      </c>
+      <c r="B68" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C68" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D68" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E68" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="251" t="s">
+        <v>3184</v>
+      </c>
+      <c r="B69" s="248"/>
+      <c r="C69" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D69" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E69" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="251" t="s">
+        <v>3230</v>
+      </c>
+      <c r="B70" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C70" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D70" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -57785,6 +60189,9 @@
     <hyperlink ref="A64" r:id="rId64"/>
     <hyperlink ref="A65" r:id="rId65"/>
     <hyperlink ref="A67" r:id="rId66"/>
+    <hyperlink ref="A68" r:id="rId67"/>
+    <hyperlink ref="A69" r:id="rId68"/>
+    <hyperlink ref="A70" r:id="rId69"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -57795,7 +60202,7 @@
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B29" sqref="B29:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58263,6 +60670,55 @@
         <v>21</v>
       </c>
       <c r="E28" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="251" t="s">
+        <v>3148</v>
+      </c>
+      <c r="B29" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C29" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D29" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E29" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="251" t="s">
+        <v>3186</v>
+      </c>
+      <c r="B30" s="248"/>
+      <c r="C30" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D30" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E30" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="251" t="s">
+        <v>3232</v>
+      </c>
+      <c r="B31" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C31" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D31" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -58351,6 +60807,9 @@
     <hyperlink ref="A24" r:id="rId25"/>
     <hyperlink ref="A25" r:id="rId26"/>
     <hyperlink ref="A28" r:id="rId27"/>
+    <hyperlink ref="A29" r:id="rId28"/>
+    <hyperlink ref="A30" r:id="rId29"/>
+    <hyperlink ref="A31" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -58358,10 +60817,10 @@
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41:E45"/>
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59496,6 +61955,55 @@
         <v>21</v>
       </c>
       <c r="E67" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="251" t="s">
+        <v>3147</v>
+      </c>
+      <c r="B68" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C68" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D68" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E68" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="251" t="s">
+        <v>3185</v>
+      </c>
+      <c r="B69" s="248"/>
+      <c r="C69" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D69" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E69" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="251" t="s">
+        <v>3231</v>
+      </c>
+      <c r="B70" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C70" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D70" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -59568,6 +62076,9 @@
     <hyperlink ref="A65" r:id="rId65"/>
     <hyperlink ref="A66" r:id="rId66"/>
     <hyperlink ref="A67" r:id="rId67"/>
+    <hyperlink ref="A68" r:id="rId68"/>
+    <hyperlink ref="A69" r:id="rId69"/>
+    <hyperlink ref="A70" r:id="rId70"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -59575,10 +62086,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41:E45"/>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85:E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60995,6 +63506,55 @@
         <v>21</v>
       </c>
       <c r="E84" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="233" t="s">
+        <v>3102</v>
+      </c>
+      <c r="B85" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C85" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D85" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E85" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="246" t="s">
+        <v>3115</v>
+      </c>
+      <c r="B86" s="248"/>
+      <c r="C86" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D86" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E86" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="251" t="s">
+        <v>3190</v>
+      </c>
+      <c r="B87" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C87" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D87" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E87" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -61075,6 +63635,9 @@
     <hyperlink ref="A81" r:id="rId73"/>
     <hyperlink ref="A83" r:id="rId74"/>
     <hyperlink ref="A84" r:id="rId75"/>
+    <hyperlink ref="A85" r:id="rId76"/>
+    <hyperlink ref="A86" r:id="rId77"/>
+    <hyperlink ref="A87" r:id="rId78"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -61082,10 +63645,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E48"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87:E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62540,6 +65103,55 @@
         <v>21</v>
       </c>
       <c r="E86" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="234" t="s">
+        <v>3103</v>
+      </c>
+      <c r="B87" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C87" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D87" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E87" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="247" t="s">
+        <v>3116</v>
+      </c>
+      <c r="B88" s="248"/>
+      <c r="C88" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D88" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E88" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="251" t="s">
+        <v>3191</v>
+      </c>
+      <c r="B89" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C89" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D89" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E89" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -62625,18 +65237,21 @@
     <hyperlink ref="A83" r:id="rId78"/>
     <hyperlink ref="A85" r:id="rId79"/>
     <hyperlink ref="A86" r:id="rId80"/>
+    <hyperlink ref="A87" r:id="rId81"/>
+    <hyperlink ref="A88" r:id="rId82"/>
+    <hyperlink ref="A89" r:id="rId83"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId81"/>
+  <pageSetup orientation="portrait" r:id="rId84"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E48"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86:E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64074,6 +66689,55 @@
         <v>21</v>
       </c>
       <c r="E85" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="235" t="s">
+        <v>3104</v>
+      </c>
+      <c r="B86" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C86" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D86" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E86" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="251" t="s">
+        <v>3117</v>
+      </c>
+      <c r="B87" s="248"/>
+      <c r="C87" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D87" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E87" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="251" t="s">
+        <v>3192</v>
+      </c>
+      <c r="B88" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C88" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D88" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E88" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -64157,6 +66821,9 @@
     <hyperlink ref="A82" r:id="rId76"/>
     <hyperlink ref="A84" r:id="rId77"/>
     <hyperlink ref="A85" r:id="rId78"/>
+    <hyperlink ref="A86" r:id="rId79"/>
+    <hyperlink ref="A87" r:id="rId80"/>
+    <hyperlink ref="A88" r:id="rId81"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -64164,10 +66831,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E48"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85:E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -65588,6 +68255,55 @@
         <v>21</v>
       </c>
       <c r="E84" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="229" t="s">
+        <v>3098</v>
+      </c>
+      <c r="B85" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C85" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D85" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E85" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="242" t="s">
+        <v>3109</v>
+      </c>
+      <c r="B86" s="248"/>
+      <c r="C86" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D86" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E86" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B87" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C87" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D87" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E87" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -65667,18 +68383,19 @@
     <hyperlink ref="A81" r:id="rId72"/>
     <hyperlink ref="A83" r:id="rId73"/>
     <hyperlink ref="A84" r:id="rId74"/>
+    <hyperlink ref="A85" r:id="rId75" display="http://www.cisco.com/web/DE/solutions/datacenter/architecture.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId75"/>
+  <pageSetup orientation="portrait" r:id="rId76"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E48"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86:E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67116,6 +69833,55 @@
         <v>21</v>
       </c>
       <c r="E85" s="217" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="237" t="s">
+        <v>3106</v>
+      </c>
+      <c r="B86" s="239" t="s">
+        <v>3233</v>
+      </c>
+      <c r="C86" s="239" t="s">
+        <v>3234</v>
+      </c>
+      <c r="D86" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E86" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="240" t="s">
+        <v>3107</v>
+      </c>
+      <c r="B87" s="248"/>
+      <c r="C87" s="238" t="s">
+        <v>3110</v>
+      </c>
+      <c r="D87" s="239" t="s">
+        <v>3111</v>
+      </c>
+      <c r="E87" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="251" t="s">
+        <v>3193</v>
+      </c>
+      <c r="B88" s="248" t="s">
+        <v>3236</v>
+      </c>
+      <c r="C88" s="248" t="s">
+        <v>3235</v>
+      </c>
+      <c r="D88" s="248" t="s">
+        <v>21</v>
+      </c>
+      <c r="E88" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -67196,6 +69962,9 @@
     <hyperlink ref="A81" r:id="rId73"/>
     <hyperlink ref="A84" r:id="rId74"/>
     <hyperlink ref="A85" r:id="rId75"/>
+    <hyperlink ref="A86" r:id="rId76"/>
+    <hyperlink ref="A87" r:id="rId77"/>
+    <hyperlink ref="A88" r:id="rId78"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated the ovwdemo 48 url excel sheet
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
+++ b/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW-jan25\OVWMigration\docs\OVW Sheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11010" firstSheet="34" activeTab="47"/>
   </bookViews>
   <sheets>
     <sheet name="ja_jp" sheetId="48" r:id="rId1"/>
@@ -61,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16117" uniqueCount="3237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16317" uniqueCount="3277">
   <si>
     <t>products</t>
   </si>
@@ -9772,6 +9777,126 @@
   </si>
   <si>
     <t>overview-WebVar3</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/produtos/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FR/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/LA/productos/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/ar/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/cisco/web/UK/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CN/products/products_netsol/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/product/hs/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/products/security/products_fr.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ANZ/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IN/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/KR/products/pc/vpndevc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/SG/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/NO/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PL/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PT/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ZA/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ES/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/SE/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CH/fr/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CH/de/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TR/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/UA/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/HK/tc/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/HK/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TW/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/EA/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IL/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/nl/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DK/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/EA/products/FR/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IT/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/NL/producten/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TH/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/AT/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/fr/products/security/products.html</t>
   </si>
 </sst>
 </file>
@@ -10303,6 +10428,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -10562,7 +10690,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10570,10 +10698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11990,6 +12118,23 @@
         <v>21</v>
       </c>
       <c r="E84" s="248" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="248" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="19" t="s">
+        <v>3245</v>
+      </c>
+      <c r="B85" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C85" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D85" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -12070,18 +12215,19 @@
     <hyperlink ref="A82" r:id="rId73"/>
     <hyperlink ref="A83" r:id="rId74"/>
     <hyperlink ref="A84" r:id="rId75"/>
+    <hyperlink ref="A85" r:id="rId76"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId76"/>
+  <pageSetup orientation="portrait" r:id="rId77"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85:E87"/>
+      <selection activeCell="B88" sqref="B88:E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13551,6 +13697,23 @@
         <v>21</v>
       </c>
       <c r="E87" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="250" t="s">
+        <v>3246</v>
+      </c>
+      <c r="B88" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D88" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -13636,6 +13799,7 @@
     <hyperlink ref="A85" r:id="rId78"/>
     <hyperlink ref="A86" r:id="rId79"/>
     <hyperlink ref="A87" r:id="rId80"/>
+    <hyperlink ref="A88" r:id="rId81"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13643,10 +13807,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86:E88"/>
+    <sheetView topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89:E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15132,6 +15296,23 @@
         <v>21</v>
       </c>
       <c r="E88" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="251" t="s">
+        <v>3247</v>
+      </c>
+      <c r="B89" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D89" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -15218,6 +15399,7 @@
     <hyperlink ref="A86" r:id="rId79"/>
     <hyperlink ref="A87" r:id="rId80"/>
     <hyperlink ref="A88" r:id="rId81"/>
+    <hyperlink ref="A89" r:id="rId82"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15225,10 +15407,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85:E87"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88:E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16694,6 +16876,23 @@
         <v>21</v>
       </c>
       <c r="E87" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="251" t="s">
+        <v>3248</v>
+      </c>
+      <c r="B88" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D88" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -16777,6 +16976,7 @@
     <hyperlink ref="A85" r:id="rId76"/>
     <hyperlink ref="A86" r:id="rId77"/>
     <hyperlink ref="A87" r:id="rId78"/>
+    <hyperlink ref="A88" r:id="rId79"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16784,10 +16984,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87:E89"/>
+      <selection activeCell="B90" sqref="B90:E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18290,6 +18490,23 @@
         <v>21</v>
       </c>
       <c r="E89" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="250" t="s">
+        <v>3249</v>
+      </c>
+      <c r="B90" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D90" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -18377,18 +18594,19 @@
     <hyperlink ref="A87" r:id="rId80"/>
     <hyperlink ref="A88" r:id="rId81"/>
     <hyperlink ref="A89" r:id="rId82"/>
+    <hyperlink ref="A90" r:id="rId83"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId83"/>
+  <pageSetup orientation="portrait" r:id="rId84"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87:E89"/>
+      <selection activeCell="B90" sqref="B90:E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19891,6 +20109,23 @@
         <v>21</v>
       </c>
       <c r="E89" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="250" t="s">
+        <v>3250</v>
+      </c>
+      <c r="B90" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D90" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -19977,6 +20212,7 @@
     <hyperlink ref="A87" r:id="rId79"/>
     <hyperlink ref="A88" r:id="rId80"/>
     <hyperlink ref="A89" r:id="rId81"/>
+    <hyperlink ref="A90" r:id="rId82"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19984,10 +20220,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72:E74"/>
+      <selection activeCell="B75" sqref="B75:E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21235,6 +21471,23 @@
         <v>21</v>
       </c>
       <c r="E74" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="250" t="s">
+        <v>3251</v>
+      </c>
+      <c r="B75" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D75" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -21312,6 +21565,7 @@
     <hyperlink ref="A72" r:id="rId70"/>
     <hyperlink ref="A73" r:id="rId71"/>
     <hyperlink ref="A74" r:id="rId72"/>
+    <hyperlink ref="A75" r:id="rId73"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21322,7 +21576,7 @@
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70:E72"/>
+      <selection activeCell="B73" sqref="B73:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22544,10 +22798,21 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="206"/>
-      <c r="B73" s="215"/>
-      <c r="C73" s="215"/>
-      <c r="D73" s="215"/>
+      <c r="A73" s="251" t="s">
+        <v>3252</v>
+      </c>
+      <c r="B73" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D73" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="249" t="s">
+        <v>2075</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="206"/>
@@ -22627,6 +22892,7 @@
     <hyperlink ref="A70" r:id="rId68"/>
     <hyperlink ref="A71" r:id="rId69"/>
     <hyperlink ref="A72" r:id="rId70"/>
+    <hyperlink ref="A73" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22634,10 +22900,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71:E73"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23864,6 +24130,23 @@
         <v>21</v>
       </c>
       <c r="E73" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="251" t="s">
+        <v>3253</v>
+      </c>
+      <c r="B74" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D74" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -23939,6 +24222,7 @@
     <hyperlink ref="A71" r:id="rId68"/>
     <hyperlink ref="A72" r:id="rId69"/>
     <hyperlink ref="A73" r:id="rId70"/>
+    <hyperlink ref="A74" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -23946,10 +24230,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70:E72"/>
+    <sheetView topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25164,6 +25448,23 @@
         <v>21</v>
       </c>
       <c r="E72" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="250" t="s">
+        <v>3254</v>
+      </c>
+      <c r="B73" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D73" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -25241,6 +25542,7 @@
     <hyperlink ref="A70" r:id="rId70"/>
     <hyperlink ref="A71" r:id="rId71"/>
     <hyperlink ref="A72" r:id="rId72"/>
+    <hyperlink ref="A73" r:id="rId73"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -25251,7 +25553,7 @@
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:E23"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25723,7 +26025,7 @@
   <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83:E83"/>
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27111,11 +27413,22 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="248"/>
-      <c r="C83" s="248"/>
-      <c r="D83" s="248"/>
-      <c r="E83" s="249"/>
+    <row r="83" spans="1:5" s="248" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="181" t="s">
+        <v>3244</v>
+      </c>
+      <c r="B83" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C83" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D83" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" s="249" t="s">
+        <v>2075</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -27193,6 +27506,7 @@
     <hyperlink ref="A80" r:id="rId72"/>
     <hyperlink ref="A81" r:id="rId73"/>
     <hyperlink ref="A82" r:id="rId74"/>
+    <hyperlink ref="A83" r:id="rId75"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -27200,10 +27514,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65:E67"/>
+      <selection activeCell="B68" sqref="B68:E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28332,6 +28646,23 @@
         <v>21</v>
       </c>
       <c r="E67" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="251" t="s">
+        <v>3255</v>
+      </c>
+      <c r="B68" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D68" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -28395,6 +28726,7 @@
     <hyperlink ref="A65" r:id="rId56"/>
     <hyperlink ref="A66" r:id="rId57"/>
     <hyperlink ref="A67" r:id="rId58"/>
+    <hyperlink ref="A68" r:id="rId59"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28402,10 +28734,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71:E73"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29631,6 +29963,23 @@
         <v>21</v>
       </c>
       <c r="E73" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="250" t="s">
+        <v>3256</v>
+      </c>
+      <c r="B74" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D74" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -29707,6 +30056,7 @@
     <hyperlink ref="A71" r:id="rId69"/>
     <hyperlink ref="A72" r:id="rId70"/>
     <hyperlink ref="A73" r:id="rId71"/>
+    <hyperlink ref="A74" r:id="rId72"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29714,10 +30064,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70:E72"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30932,6 +31282,23 @@
         <v>21</v>
       </c>
       <c r="E72" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="251" t="s">
+        <v>3257</v>
+      </c>
+      <c r="B73" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D73" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -31008,6 +31375,7 @@
     <hyperlink ref="A70" r:id="rId69"/>
     <hyperlink ref="A71" r:id="rId70"/>
     <hyperlink ref="A72" r:id="rId71"/>
+    <hyperlink ref="A73" r:id="rId72"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -31015,10 +31383,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69:E71"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72:E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32216,6 +32584,23 @@
         <v>21</v>
       </c>
       <c r="E71" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="250" t="s">
+        <v>3258</v>
+      </c>
+      <c r="B72" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -32291,6 +32676,7 @@
     <hyperlink ref="A69" r:id="rId68"/>
     <hyperlink ref="A70" r:id="rId69"/>
     <hyperlink ref="A71" r:id="rId70"/>
+    <hyperlink ref="A72" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -32298,10 +32684,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69:E71"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72:E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33499,6 +33885,23 @@
         <v>21</v>
       </c>
       <c r="E71" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="250" t="s">
+        <v>3259</v>
+      </c>
+      <c r="B72" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -33575,6 +33978,7 @@
     <hyperlink ref="A69" r:id="rId69"/>
     <hyperlink ref="A70" r:id="rId70"/>
     <hyperlink ref="A71" r:id="rId71"/>
+    <hyperlink ref="A72" r:id="rId72"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33582,10 +33986,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71:E73"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34811,6 +35215,23 @@
         <v>21</v>
       </c>
       <c r="E73" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="251" t="s">
+        <v>3260</v>
+      </c>
+      <c r="B74" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D74" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -34887,6 +35308,7 @@
     <hyperlink ref="A71" r:id="rId69"/>
     <hyperlink ref="A72" r:id="rId70"/>
     <hyperlink ref="A73" r:id="rId71"/>
+    <hyperlink ref="A74" r:id="rId72"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34894,10 +35316,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67:E68"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69:E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36038,6 +36460,23 @@
         <v>21</v>
       </c>
       <c r="E68" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="251" t="s">
+        <v>3261</v>
+      </c>
+      <c r="B69" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D69" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -36109,6 +36548,7 @@
     <hyperlink ref="A66" r:id="rId64"/>
     <hyperlink ref="A67" r:id="rId65"/>
     <hyperlink ref="A68" r:id="rId66"/>
+    <hyperlink ref="A69" r:id="rId67"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -36528,10 +36968,10 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69:E71"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72:E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37726,6 +38166,23 @@
         <v>21</v>
       </c>
       <c r="E71" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="199" t="s">
+        <v>3262</v>
+      </c>
+      <c r="B72" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -37799,6 +38256,7 @@
     <hyperlink ref="A68" r:id="rId66"/>
     <hyperlink ref="A69" r:id="rId67"/>
     <hyperlink ref="A71" r:id="rId68"/>
+    <hyperlink ref="A72" r:id="rId69"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -37806,10 +38264,10 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71:E73"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39035,6 +39493,23 @@
         <v>21</v>
       </c>
       <c r="E73" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="250" t="s">
+        <v>3263</v>
+      </c>
+      <c r="B74" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D74" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -39111,6 +39586,7 @@
     <hyperlink ref="A71" r:id="rId69"/>
     <hyperlink ref="A72" r:id="rId70"/>
     <hyperlink ref="A73" r:id="rId71"/>
+    <hyperlink ref="A74" r:id="rId72"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -39118,10 +39594,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87:E87"/>
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40590,6 +41066,23 @@
         <v>21</v>
       </c>
       <c r="E87" s="248" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="248" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="181" t="s">
+        <v>3243</v>
+      </c>
+      <c r="B88" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D88" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -40675,6 +41168,7 @@
     <hyperlink ref="A85" r:id="rId78"/>
     <hyperlink ref="A86" r:id="rId79"/>
     <hyperlink ref="A87" r:id="rId80"/>
+    <hyperlink ref="A88" r:id="rId81"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -40682,10 +41176,10 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71:E73"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41911,6 +42405,23 @@
         <v>21</v>
       </c>
       <c r="E73" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="251" t="s">
+        <v>3264</v>
+      </c>
+      <c r="B74" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D74" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -41987,6 +42498,7 @@
     <hyperlink ref="A71" r:id="rId69"/>
     <hyperlink ref="A72" r:id="rId70"/>
     <hyperlink ref="A73" r:id="rId71"/>
+    <hyperlink ref="A74" r:id="rId72"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -41994,10 +42506,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68:E70"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43181,6 +43693,23 @@
         <v>21</v>
       </c>
       <c r="E70" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="251" t="s">
+        <v>3265</v>
+      </c>
+      <c r="B71" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D71" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -43256,6 +43785,7 @@
     <hyperlink ref="A68" r:id="rId68"/>
     <hyperlink ref="A69" r:id="rId69"/>
     <hyperlink ref="A70" r:id="rId70"/>
+    <hyperlink ref="A71" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -43265,8 +43795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66:E67"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68:E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44400,10 +44930,21 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="248"/>
-      <c r="C68" s="248"/>
-      <c r="D68" s="248"/>
-      <c r="E68" s="249"/>
+      <c r="A68" s="251" t="s">
+        <v>3266</v>
+      </c>
+      <c r="B68" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D68" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="249" t="s">
+        <v>2075</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -44473,6 +45014,7 @@
     <hyperlink ref="A65" r:id="rId64"/>
     <hyperlink ref="A66" r:id="rId65"/>
     <hyperlink ref="A67" r:id="rId66"/>
+    <hyperlink ref="A68" r:id="rId67"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -44895,10 +45437,10 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70:E72"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46116,6 +46658,23 @@
         <v>21</v>
       </c>
       <c r="E72" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="250" t="s">
+        <v>3267</v>
+      </c>
+      <c r="B73" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D73" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -46192,6 +46751,7 @@
     <hyperlink ref="A70" r:id="rId69"/>
     <hyperlink ref="A71" r:id="rId70"/>
     <hyperlink ref="A72" r:id="rId71"/>
+    <hyperlink ref="A73" r:id="rId72"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -47454,10 +48014,10 @@
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71:E73"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48692,6 +49252,23 @@
         <v>21</v>
       </c>
       <c r="E73" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="251" t="s">
+        <v>3268</v>
+      </c>
+      <c r="B74" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D74" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -48767,6 +49344,7 @@
     <hyperlink ref="A71" r:id="rId68"/>
     <hyperlink ref="A72" r:id="rId69"/>
     <hyperlink ref="A73" r:id="rId70"/>
+    <hyperlink ref="A74" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -48774,10 +49352,10 @@
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70:E72"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49995,6 +50573,23 @@
         <v>21</v>
       </c>
       <c r="E72" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="250" t="s">
+        <v>3269</v>
+      </c>
+      <c r="B73" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D73" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -50072,6 +50667,7 @@
     <hyperlink ref="A70" r:id="rId70"/>
     <hyperlink ref="A71" r:id="rId71"/>
     <hyperlink ref="A72" r:id="rId72"/>
+    <hyperlink ref="A73" r:id="rId73"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -50079,10 +50675,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88:E88"/>
+      <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51568,6 +52164,23 @@
         <v>21</v>
       </c>
       <c r="E88" s="248" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="248" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="181" t="s">
+        <v>3242</v>
+      </c>
+      <c r="B89" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D89" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -51652,6 +52265,7 @@
     <hyperlink ref="A86" r:id="rId77"/>
     <hyperlink ref="A87" r:id="rId78"/>
     <hyperlink ref="A88" r:id="rId79"/>
+    <hyperlink ref="A89" r:id="rId80"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -52068,10 +52682,10 @@
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72:E74"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75:E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53325,6 +53939,23 @@
         <v>21</v>
       </c>
       <c r="E74" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="250" t="s">
+        <v>3270</v>
+      </c>
+      <c r="B75" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D75" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -53404,6 +54035,7 @@
     <hyperlink ref="A72" r:id="rId72"/>
     <hyperlink ref="A73" r:id="rId73"/>
     <hyperlink ref="A74" r:id="rId74"/>
+    <hyperlink ref="A75" r:id="rId75"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -53411,10 +54043,10 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86:E88"/>
+      <selection activeCell="B89" sqref="B89:E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54900,6 +55532,23 @@
         <v>21</v>
       </c>
       <c r="E88" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="250" t="s">
+        <v>3271</v>
+      </c>
+      <c r="B89" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D89" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -54985,6 +55634,7 @@
     <hyperlink ref="A86" r:id="rId78"/>
     <hyperlink ref="A87" r:id="rId79"/>
     <hyperlink ref="A88" r:id="rId80"/>
+    <hyperlink ref="A89" r:id="rId81"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -54992,10 +55642,10 @@
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72:E74"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75:E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56243,6 +56893,23 @@
         <v>21</v>
       </c>
       <c r="E74" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="199" t="s">
+        <v>3272</v>
+      </c>
+      <c r="B75" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D75" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -56320,6 +56987,7 @@
     <hyperlink ref="A72" r:id="rId70"/>
     <hyperlink ref="A73" r:id="rId71"/>
     <hyperlink ref="A74" r:id="rId72"/>
+    <hyperlink ref="A75" r:id="rId73"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -56327,10 +56995,10 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72:E74"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75:E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57578,6 +58246,23 @@
         <v>21</v>
       </c>
       <c r="E74" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="250" t="s">
+        <v>3273</v>
+      </c>
+      <c r="B75" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D75" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -57655,6 +58340,7 @@
     <hyperlink ref="A72" r:id="rId70"/>
     <hyperlink ref="A73" r:id="rId71"/>
     <hyperlink ref="A74" r:id="rId72"/>
+    <hyperlink ref="A75" r:id="rId73"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -57662,10 +58348,10 @@
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68:E70"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58849,6 +59535,23 @@
         <v>21</v>
       </c>
       <c r="E70" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="250" t="s">
+        <v>3274</v>
+      </c>
+      <c r="B71" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D71" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -58924,6 +59627,7 @@
     <hyperlink ref="A68" r:id="rId68"/>
     <hyperlink ref="A69" r:id="rId69"/>
     <hyperlink ref="A70" r:id="rId70"/>
+    <hyperlink ref="A71" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -58931,10 +59635,10 @@
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68:E70"/>
+    <sheetView topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60118,6 +60822,23 @@
         <v>21</v>
       </c>
       <c r="E70" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="251" t="s">
+        <v>3275</v>
+      </c>
+      <c r="B71" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D71" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -60192,6 +60913,7 @@
     <hyperlink ref="A68" r:id="rId67"/>
     <hyperlink ref="A69" r:id="rId68"/>
     <hyperlink ref="A70" r:id="rId69"/>
+    <hyperlink ref="A71" r:id="rId70"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -60817,10 +61539,10 @@
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62004,6 +62726,23 @@
         <v>21</v>
       </c>
       <c r="E70" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="251" t="s">
+        <v>3276</v>
+      </c>
+      <c r="B71" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D71" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -62079,6 +62818,7 @@
     <hyperlink ref="A68" r:id="rId68"/>
     <hyperlink ref="A69" r:id="rId69"/>
     <hyperlink ref="A70" r:id="rId70"/>
+    <hyperlink ref="A71" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -62086,10 +62826,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87:E87"/>
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63555,6 +64295,23 @@
         <v>21</v>
       </c>
       <c r="E87" s="248" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="248" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="181" t="s">
+        <v>3240</v>
+      </c>
+      <c r="B88" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D88" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -63638,6 +64395,7 @@
     <hyperlink ref="A85" r:id="rId76"/>
     <hyperlink ref="A86" r:id="rId77"/>
     <hyperlink ref="A87" r:id="rId78"/>
+    <hyperlink ref="A88" r:id="rId79"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -63645,10 +64403,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89:E89"/>
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -65152,6 +65910,23 @@
         <v>21</v>
       </c>
       <c r="E89" s="248" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" s="248" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="19" t="s">
+        <v>3237</v>
+      </c>
+      <c r="B90" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D90" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -65240,18 +66015,19 @@
     <hyperlink ref="A87" r:id="rId81"/>
     <hyperlink ref="A88" r:id="rId82"/>
     <hyperlink ref="A89" r:id="rId83"/>
+    <hyperlink ref="A90" r:id="rId84"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId84"/>
+  <pageSetup orientation="portrait" r:id="rId85"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88:E88"/>
+      <selection activeCell="A90" sqref="A90:XFD90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -66740,6 +67516,27 @@
       <c r="E88" s="248" t="s">
         <v>2075</v>
       </c>
+    </row>
+    <row r="89" spans="1:5" s="248" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="19" t="s">
+        <v>3241</v>
+      </c>
+      <c r="B89" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D89" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="249" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" s="248" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="181"/>
+      <c r="E90" s="249"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -66824,6 +67621,7 @@
     <hyperlink ref="A86" r:id="rId79"/>
     <hyperlink ref="A87" r:id="rId80"/>
     <hyperlink ref="A88" r:id="rId81"/>
+    <hyperlink ref="A89" r:id="rId82"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -66831,10 +67629,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87:E87"/>
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -68304,6 +69102,23 @@
         <v>21</v>
       </c>
       <c r="E87" s="248" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="248" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="19" t="s">
+        <v>3238</v>
+      </c>
+      <c r="B88" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D88" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -68384,18 +69199,19 @@
     <hyperlink ref="A83" r:id="rId73"/>
     <hyperlink ref="A84" r:id="rId74"/>
     <hyperlink ref="A85" r:id="rId75" display="http://www.cisco.com/web/DE/solutions/datacenter/architecture.html"/>
+    <hyperlink ref="A88" r:id="rId76"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId76"/>
+  <pageSetup orientation="portrait" r:id="rId77"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+      <selection activeCell="B89" sqref="B89:E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -69882,6 +70698,23 @@
         <v>21</v>
       </c>
       <c r="E88" s="248" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="248" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="19" t="s">
+        <v>3239</v>
+      </c>
+      <c r="B89" s="248" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" s="248" t="s">
+        <v>34</v>
+      </c>
+      <c r="D89" s="248" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="249" t="s">
         <v>2075</v>
       </c>
     </row>
@@ -69965,6 +70798,7 @@
     <hyperlink ref="A86" r:id="rId76"/>
     <hyperlink ref="A87" r:id="rId77"/>
     <hyperlink ref="A88" r:id="rId78"/>
+    <hyperlink ref="A89" r:id="rId79"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modified 3rd column of collaboration solution listing
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
+++ b/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW Migration\OVWMigration\docs\OVW Sheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11010" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11010"/>
   </bookViews>
   <sheets>
     <sheet name="ja_jp" sheetId="48" r:id="rId1"/>
@@ -61,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16529" uniqueCount="3454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16529" uniqueCount="3455">
   <si>
     <t>products</t>
   </si>
@@ -10423,6 +10428,9 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/FR/products/index.html</t>
+  </si>
+  <si>
+    <t>solution-listing-var6</t>
   </si>
 </sst>
 </file>
@@ -11665,7 +11673,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -11675,8 +11683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12000,7 +12008,7 @@
         <v>26</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>21</v>
@@ -13252,7 +13260,7 @@
   <dimension ref="A1:F91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13338,7 +13346,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="78" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="78" t="s">
         <v>21</v>
@@ -13705,7 +13713,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="151" t="s">
         <v>1209</v>
       </c>
@@ -13722,7 +13730,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="151" t="s">
         <v>1211</v>
       </c>
@@ -13739,7 +13747,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="151" t="s">
         <v>1212</v>
       </c>
@@ -13756,7 +13764,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="151" t="s">
         <v>1213</v>
       </c>
@@ -13773,7 +13781,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="150" t="s">
         <v>1215</v>
       </c>
@@ -13790,7 +13798,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="176" t="s">
         <v>1593</v>
       </c>
@@ -13807,7 +13815,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="176" t="s">
         <v>1595</v>
       </c>
@@ -13824,7 +13832,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="176" t="s">
         <v>1596</v>
       </c>
@@ -13841,7 +13849,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="176" t="s">
         <v>1597</v>
       </c>
@@ -14884,8 +14892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14971,7 +14979,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="81" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="81" t="s">
         <v>21</v>
@@ -16535,7 +16543,7 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16571,7 +16579,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="75" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D2" s="75" t="s">
         <v>21</v>
@@ -16988,7 +16996,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="172" t="s">
         <v>1546</v>
       </c>
@@ -17005,7 +17013,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="171" t="s">
         <v>1548</v>
       </c>
@@ -17022,7 +17030,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="190" t="s">
         <v>1740</v>
       </c>
@@ -17039,7 +17047,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="190" t="s">
         <v>1742</v>
       </c>
@@ -17056,7 +17064,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="190" t="s">
         <v>1743</v>
       </c>
@@ -17073,7 +17081,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="191" t="s">
         <v>1744</v>
       </c>
@@ -18134,7 +18142,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18169,7 +18177,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D2" s="194" t="s">
         <v>21</v>
@@ -19420,7 +19428,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19455,7 +19463,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D2" s="194" t="s">
         <v>21</v>
@@ -20705,7 +20713,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:E53"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20740,7 +20748,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D2" s="194" t="s">
         <v>21</v>
@@ -21991,7 +21999,7 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:E61"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22077,7 +22085,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -23311,8 +23319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:E38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23399,7 +23407,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -24614,7 +24622,7 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24701,7 +24709,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -25915,7 +25923,7 @@
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26001,7 +26009,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -27252,7 +27260,7 @@
   <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27577,7 +27585,7 @@
         <v>26</v>
       </c>
       <c r="C19" s="53" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D19" s="53" t="s">
         <v>21</v>
@@ -28794,7 +28802,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28880,7 +28888,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -30078,8 +30086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30166,7 +30174,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -31409,7 +31417,7 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31496,7 +31504,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -32721,7 +32729,7 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32825,7 +32833,7 @@
         <v>26</v>
       </c>
       <c r="C6" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D6" s="194" t="s">
         <v>21</v>
@@ -33174,7 +33182,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="174" t="s">
         <v>1323</v>
       </c>
@@ -33191,7 +33199,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="174" t="s">
         <v>1324</v>
       </c>
@@ -33208,7 +33216,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="164" t="s">
         <v>1325</v>
       </c>
@@ -33225,7 +33233,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="174" t="s">
         <v>1326</v>
       </c>
@@ -33242,7 +33250,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="174" t="s">
         <v>1327</v>
       </c>
@@ -33259,7 +33267,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="174" t="s">
         <v>1328</v>
       </c>
@@ -33276,7 +33284,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="174" t="s">
         <v>1329</v>
       </c>
@@ -33293,7 +33301,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="174" t="s">
         <v>1330</v>
       </c>
@@ -33310,7 +33318,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="164" t="s">
         <v>1331</v>
       </c>
@@ -34034,8 +34042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34105,7 +34113,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D4" s="194" t="s">
         <v>21</v>
@@ -35267,7 +35275,7 @@
   <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35353,7 +35361,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="86" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="86" t="s">
         <v>21</v>
@@ -35719,7 +35727,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="160" t="s">
         <v>1356</v>
       </c>
@@ -35736,7 +35744,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="160" t="s">
         <v>1358</v>
       </c>
@@ -35753,7 +35761,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="160" t="s">
         <v>1359</v>
       </c>
@@ -35770,7 +35778,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="160" t="s">
         <v>1360</v>
       </c>
@@ -35787,7 +35795,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="159" t="s">
         <v>1362</v>
       </c>
@@ -36935,8 +36943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37022,7 +37030,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="89" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="89" t="s">
         <v>21</v>
@@ -38602,8 +38610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:E56"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38689,7 +38697,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="91" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="91" t="s">
         <v>21</v>
@@ -39954,7 +39962,7 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A64" sqref="A64:E64"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40040,7 +40048,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -41277,7 +41285,7 @@
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41365,7 +41373,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -42607,7 +42615,7 @@
   <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42948,7 +42956,7 @@
         <v>26</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D20" s="46" t="s">
         <v>21</v>
@@ -43059,7 +43067,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="48" t="s">
         <v>351</v>
       </c>
@@ -44239,7 +44247,7 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44326,7 +44334,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -45564,7 +45572,7 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45616,7 +45624,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D3" s="194" t="s">
         <v>21</v>
@@ -46035,7 +46043,7 @@
   <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46121,7 +46129,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -47275,8 +47283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47363,7 +47371,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -48595,7 +48603,7 @@
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48682,7 +48690,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -49925,7 +49933,7 @@
   <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49995,7 +50003,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D4" s="194" t="s">
         <v>21</v>
@@ -51167,7 +51175,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51219,7 +51227,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D3" s="194" t="s">
         <v>21</v>
@@ -51592,7 +51600,7 @@
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51679,7 +51687,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -52922,7 +52930,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52974,7 +52982,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D3" s="194" t="s">
         <v>21</v>
@@ -53350,7 +53358,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53402,7 +53410,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D3" s="194" t="s">
         <v>21</v>
@@ -53777,8 +53785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54119,7 +54127,7 @@
         <v>26</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D20" s="39" t="s">
         <v>21</v>
@@ -55426,7 +55434,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55478,7 +55486,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D3" s="194" t="s">
         <v>21</v>
@@ -55870,7 +55878,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55922,7 +55930,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D3" s="194" t="s">
         <v>21</v>
@@ -56298,7 +56306,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A64" sqref="A64:E64"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56384,7 +56392,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -57587,7 +57595,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57639,7 +57647,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D3" s="194" t="s">
         <v>21</v>
@@ -58014,7 +58022,7 @@
   <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:E56"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58100,7 +58108,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -59374,7 +59382,7 @@
   <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59460,7 +59468,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -61023,7 +61031,7 @@
   <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61109,7 +61117,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -62373,7 +62381,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -62458,7 +62468,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D5" s="194" t="s">
         <v>21</v>
@@ -63722,8 +63732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63792,7 +63802,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="83" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D4" s="83" t="s">
         <v>21</v>
@@ -64359,8 +64369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:E61"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64701,7 +64711,7 @@
         <v>26</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>21</v>
@@ -66048,7 +66058,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -66389,7 +66401,7 @@
         <v>26</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>21</v>
@@ -67718,7 +67730,7 @@
   <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -68060,7 +68072,7 @@
         <v>26</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D20" s="33" t="s">
         <v>21</v>
@@ -68171,7 +68183,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="34" t="s">
         <v>267</v>
       </c>
@@ -69368,8 +69380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -69694,7 +69706,7 @@
         <v>26</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>21</v>
@@ -70997,8 +71009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -71323,7 +71335,7 @@
         <v>26</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>47</v>
+        <v>3454</v>
       </c>
       <c r="D19" s="21" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
updated the all url excel sheet
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
+++ b/docs/OVW Sheets/OVWDemo_ALL_URLS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW feb 15 new\OVWMigration\docs\OVW Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW feb 16\OVWMigration\docs\OVW Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16490" uniqueCount="3454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16489" uniqueCount="3454">
   <si>
     <t>products</t>
   </si>
@@ -63663,8 +63663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64207,9 +64207,7 @@
       <c r="D55" s="194" t="s">
         <v>0</v>
       </c>
-      <c r="E55" s="194" t="s">
-        <v>2070</v>
-      </c>
+      <c r="E55" s="194"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="194" t="s">

</xml_diff>